<commit_message>
Makes changes to the 'Repo' section.
Adds the 'git prune' command.
Removes the 2 incorrect 'prune' commands from 'git remote' list.
Removes the duplicate 'git remote' from the 'Update a repo' command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-shortcuts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D255D9-1093-5E4C-923F-2D5DD4FB27CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AE92E6-B5B2-884B-8D29-195D1CF83BAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13000" yWindow="460" windowWidth="34960" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1284" uniqueCount="664">
   <si>
     <t>Configuration</t>
   </si>
@@ -2486,12 +2486,6 @@
     </r>
   </si>
   <si>
-    <t>Remove (delete) an orphaned tracking branch</t>
-  </si>
-  <si>
-    <t>Preview deletion of an orphaned tracking branch</t>
-  </si>
-  <si>
     <r>
       <t>git fetch (</t>
     </r>
@@ -2543,129 +2537,6 @@
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve">-p </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --prune</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>origin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve">-p </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --prune</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>origin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --dry-run</t>
     </r>
   </si>
   <si>
@@ -9838,29 +9709,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> branch name (recommended)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git remote </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>origin</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> remote_url</t>
     </r>
   </si>
   <si>
@@ -10341,6 +10189,70 @@
         <family val="2"/>
       </rPr>
       <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>git prune</t>
+  </si>
+  <si>
+    <t>Remove (delete) an orphaned branch</t>
+  </si>
+  <si>
+    <t>(-n OR --dry-run)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Preview</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> removal of an orphaned branch</t>
+    </r>
+  </si>
+  <si>
+    <t>(-v OR --verbose)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Remove (delete) an orphaned branch with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>detailed readout</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>origin</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> remote_url</t>
     </r>
   </si>
 </sst>
@@ -10795,12 +10707,12 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11121,8 +11033,8 @@
   </sheetPr>
   <dimension ref="A1:G446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="190" zoomScaleNormal="190" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A352" zoomScale="168" zoomScaleNormal="168" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="A352" sqref="A352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11137,83 +11049,83 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31">
       <c r="A1" s="17" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="18" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -11221,25 +11133,25 @@
         <v>44</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -11248,12 +11160,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="1" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -11262,12 +11174,12 @@
         <v>2</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="13" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>5</v>
@@ -11276,7 +11188,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -11287,12 +11199,12 @@
         <v>4</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="32" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -11306,7 +11218,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -11320,7 +11232,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -11331,10 +11243,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -11345,10 +11257,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>660</v>
+        <v>655</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>661</v>
+        <v>656</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -11359,10 +11271,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -11376,7 +11288,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -11387,10 +11299,10 @@
         <v>4</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -11401,10 +11313,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -11418,7 +11330,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -11432,7 +11344,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -11446,29 +11358,29 @@
         <v>53</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="C29" s="1" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="F29" s="14" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="33" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -11480,16 +11392,16 @@
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="21" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="33"/>
       <c r="C33" s="35" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="F33" s="31" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -11499,7 +11411,7 @@
     <row r="35" spans="1:6" ht="20" thickBot="1">
       <c r="A35" s="33"/>
       <c r="C35" s="36" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
@@ -11511,25 +11423,25 @@
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="21" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="33"/>
       <c r="C37" s="4" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="33"/>
       <c r="C38" s="39" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -11543,43 +11455,43 @@
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="21" t="s">
-        <v>622</v>
+        <v>617</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="33"/>
       <c r="C41" s="41" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="33"/>
       <c r="C42" s="4" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="33"/>
       <c r="C43" s="4" t="s">
-        <v>627</v>
+        <v>622</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>628</v>
+        <v>623</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="40">
       <c r="A44" s="33"/>
       <c r="C44" s="39" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
       <c r="F44" s="42" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -11589,10 +11501,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="33"/>
-      <c r="C46" s="55" t="s">
-        <v>631</v>
-      </c>
-      <c r="D46" s="56"/>
+      <c r="C46" s="57" t="s">
+        <v>626</v>
+      </c>
+      <c r="D46" s="58"/>
       <c r="E46" s="37"/>
       <c r="F46" s="43"/>
     </row>
@@ -11602,52 +11514,52 @@
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="46" t="s">
-        <v>632</v>
+        <v>627</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="33"/>
       <c r="C48" s="41" t="s">
-        <v>623</v>
+        <v>618</v>
       </c>
       <c r="F48" s="14" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="33"/>
       <c r="C49" s="4" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>626</v>
+        <v>621</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="33"/>
       <c r="C50" s="4" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="F50" s="14" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="40">
       <c r="A51" s="33"/>
       <c r="C51" s="39" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="F51" s="42" t="s">
-        <v>637</v>
+        <v>632</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="40">
       <c r="A52" s="33"/>
       <c r="C52" s="39" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="F52" s="42" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -11658,7 +11570,7 @@
     <row r="54" spans="1:6" ht="20" thickBot="1">
       <c r="A54" s="33"/>
       <c r="C54" s="36" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="D54" s="37"/>
       <c r="E54" s="37"/>
@@ -11670,52 +11582,52 @@
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="21" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="27">
       <c r="A56" s="33"/>
       <c r="C56" s="51" t="s">
-        <v>641</v>
+        <v>636</v>
       </c>
       <c r="F56" s="47" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="33"/>
       <c r="C57" s="39" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="F57" s="42" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="33"/>
       <c r="C58" s="39" t="s">
-        <v>644</v>
+        <v>639</v>
       </c>
       <c r="F58" s="42" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="26">
       <c r="A59" s="33"/>
       <c r="C59" s="50" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F59" s="49" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="40">
       <c r="A60" s="33"/>
       <c r="C60" s="41" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="F60" s="47" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -11729,25 +11641,25 @@
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="21" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="27">
       <c r="A63" s="33"/>
       <c r="C63" s="48" t="s">
-        <v>651</v>
+        <v>646</v>
       </c>
       <c r="F63" s="47" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="26">
       <c r="A64" s="33"/>
       <c r="C64" s="50" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -11761,25 +11673,25 @@
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="21" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="27">
       <c r="A67" s="33"/>
       <c r="C67" s="52" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="F67" s="47" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26">
       <c r="A68" s="33"/>
       <c r="C68" s="50" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -11788,21 +11700,21 @@
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="54"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="56"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -11810,15 +11722,15 @@
         <v>156</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="C73" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -11826,7 +11738,7 @@
         <v>155</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -11834,7 +11746,7 @@
         <v>10</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -11842,7 +11754,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -11850,7 +11762,7 @@
         <v>12</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -11858,7 +11770,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -11866,15 +11778,15 @@
         <v>109</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17">
       <c r="C80" s="9" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -11882,15 +11794,15 @@
         <v>51</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="C82" s="1" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -11898,7 +11810,7 @@
         <v>65</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -11906,7 +11818,7 @@
         <v>157</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -11914,28 +11826,28 @@
         <v>158</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="53" t="s">
+      <c r="A87" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="53"/>
-      <c r="C87" s="53"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="54"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="56"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -11943,7 +11855,7 @@
         <v>18</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -11951,39 +11863,39 @@
         <v>19</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="C91" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="C92" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="C93" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="C94" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -11991,7 +11903,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -11999,25 +11911,25 @@
         <v>25</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="53" t="s">
+      <c r="A98" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="53"/>
-      <c r="C98" s="53"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="53"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="55"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -12025,7 +11937,7 @@
         <v>33</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -12033,7 +11945,7 @@
         <v>182</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -12041,7 +11953,7 @@
         <v>181</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -12049,7 +11961,7 @@
         <v>22</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -12057,7 +11969,7 @@
         <v>98</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -12065,7 +11977,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -12073,15 +11985,15 @@
         <v>97</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="C107" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -12089,31 +12001,31 @@
         <v>24</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="C109" s="11" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="C110" s="11" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F110" s="14" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="C111" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -12121,7 +12033,7 @@
         <v>65</v>
       </c>
       <c r="F112" s="14" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -12129,7 +12041,7 @@
         <v>157</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -12137,26 +12049,26 @@
         <v>158</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="C116" s="13" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D116" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>4</v>
@@ -12165,12 +12077,12 @@
         <v>162</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>4</v>
@@ -12179,12 +12091,12 @@
         <v>167</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>4</v>
@@ -12193,12 +12105,12 @@
         <v>168</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>4</v>
@@ -12207,40 +12119,40 @@
         <v>161</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F122" s="14" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="13" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D124" s="13" t="s">
         <v>5</v>
@@ -12249,7 +12161,7 @@
         <v>26</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -12263,7 +12175,7 @@
         <v>64</v>
       </c>
       <c r="F125" s="14" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -12274,10 +12186,10 @@
         <v>4</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="F126" s="14" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -12291,7 +12203,7 @@
         <v>63</v>
       </c>
       <c r="F127" s="14" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -12302,10 +12214,10 @@
         <v>4</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F128" s="14" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -12319,7 +12231,7 @@
         <v>159</v>
       </c>
       <c r="F129" s="14" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -12330,36 +12242,36 @@
         <v>4</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F130" s="14" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="53" t="s">
+      <c r="A132" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="53"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="53"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="54"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="55"/>
+      <c r="E132" s="55"/>
+      <c r="F132" s="56"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F133" s="14" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="13" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D135" s="13" t="s">
         <v>5</v>
@@ -12368,7 +12280,7 @@
         <v>23</v>
       </c>
       <c r="F135" s="15" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -12379,10 +12291,10 @@
         <v>4</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F136" s="14" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -12396,7 +12308,7 @@
         <v>185</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -12410,7 +12322,7 @@
         <v>67</v>
       </c>
       <c r="F138" s="14" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -12424,7 +12336,7 @@
         <v>70</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -12438,7 +12350,7 @@
         <v>68</v>
       </c>
       <c r="F140" s="14" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -12457,7 +12369,7 @@
         <v>71</v>
       </c>
       <c r="F142" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -12471,7 +12383,7 @@
         <v>62</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -12485,7 +12397,7 @@
         <v>60</v>
       </c>
       <c r="F144" s="14" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -12499,7 +12411,7 @@
         <v>61</v>
       </c>
       <c r="F145" s="14" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -12510,10 +12422,10 @@
         <v>4</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="F146" s="14" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -12527,7 +12439,7 @@
         <v>59</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -12541,7 +12453,7 @@
         <v>58</v>
       </c>
       <c r="F148" s="14" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -12555,7 +12467,7 @@
         <v>57</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -12569,7 +12481,7 @@
         <v>56</v>
       </c>
       <c r="F150" s="14" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -12583,7 +12495,7 @@
         <v>27</v>
       </c>
       <c r="F151" s="14" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -12597,7 +12509,7 @@
         <v>66</v>
       </c>
       <c r="F152" s="14" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -12608,10 +12520,10 @@
         <v>4</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="F153" s="14" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -12625,7 +12537,7 @@
         <v>1</v>
       </c>
       <c r="F155" s="22" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -12639,7 +12551,7 @@
         <v>1</v>
       </c>
       <c r="F156" s="14" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -12653,7 +12565,7 @@
         <v>38</v>
       </c>
       <c r="F157" s="14" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -12667,7 +12579,7 @@
         <v>1</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -12681,7 +12593,7 @@
         <v>39</v>
       </c>
       <c r="F159" s="14" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -12695,7 +12607,7 @@
         <v>40</v>
       </c>
       <c r="F160" s="15" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -12709,7 +12621,7 @@
         <v>85</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -12723,7 +12635,7 @@
         <v>87</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -12734,10 +12646,10 @@
         <v>4</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -12751,7 +12663,7 @@
         <v>88</v>
       </c>
       <c r="F164" s="14" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -12765,7 +12677,7 @@
         <v>89</v>
       </c>
       <c r="F165" s="14" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -12776,10 +12688,10 @@
         <v>4</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -12793,7 +12705,7 @@
         <v>90</v>
       </c>
       <c r="F167" s="14" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -12807,7 +12719,7 @@
         <v>91</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -12818,10 +12730,10 @@
         <v>4</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="F169" s="14" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -12835,7 +12747,7 @@
         <v>92</v>
       </c>
       <c r="F170" s="14" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -12849,7 +12761,7 @@
         <v>93</v>
       </c>
       <c r="F171" s="14" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -12863,7 +12775,7 @@
         <v>94</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -12877,7 +12789,7 @@
         <v>95</v>
       </c>
       <c r="F173" s="14" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -12888,10 +12800,10 @@
         <v>4</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="F174" s="14" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -12902,10 +12814,10 @@
         <v>4</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="F175" s="14" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -12916,10 +12828,10 @@
         <v>4</v>
       </c>
       <c r="C176" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F176" s="14" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -12930,10 +12842,10 @@
         <v>4</v>
       </c>
       <c r="C177" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="F177" s="14" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -12944,99 +12856,99 @@
         <v>4</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="180" spans="1:6">
       <c r="C180" s="13" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="D180" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E180" s="13" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F180" s="21" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F181" s="14" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="F182" s="14" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="F183" s="14" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="F184" s="14" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
     </row>
     <row r="186" spans="1:6">
       <c r="C186" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="F186" s="22" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
     </row>
     <row r="187" spans="1:6">
       <c r="C187" s="26" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="D187" s="25" t="s">
         <v>5</v>
@@ -13045,21 +12957,21 @@
         <v>73</v>
       </c>
       <c r="F187" s="27" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="C188" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -13070,10 +12982,10 @@
         <v>4</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="F189" s="14" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -13084,10 +12996,10 @@
         <v>4</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="F190" s="14" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -13098,10 +13010,10 @@
         <v>4</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F191" s="14" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -13112,10 +13024,10 @@
         <v>4</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -13126,10 +13038,10 @@
         <v>4</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="F193" s="14" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -13140,31 +13052,31 @@
         <v>4</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="F194" s="14" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="53" t="s">
-        <v>433</v>
-      </c>
-      <c r="B196" s="53"/>
-      <c r="C196" s="53"/>
-      <c r="D196" s="53"/>
-      <c r="E196" s="53"/>
-      <c r="F196" s="53"/>
+      <c r="A196" s="55" t="s">
+        <v>429</v>
+      </c>
+      <c r="B196" s="55"/>
+      <c r="C196" s="55"/>
+      <c r="D196" s="55"/>
+      <c r="E196" s="55"/>
+      <c r="F196" s="55"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F197" s="28" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -13181,7 +13093,7 @@
         <v>37</v>
       </c>
       <c r="F199" s="21" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -13192,10 +13104,10 @@
         <v>4</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F200" s="14" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -13206,10 +13118,10 @@
         <v>4</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F201" s="14" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -13217,164 +13129,164 @@
     </row>
     <row r="203" spans="1:6">
       <c r="C203" s="24" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D203" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E203" s="13" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="F203" s="21" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F204" s="14" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F205" s="14" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F206" s="14" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E207" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="F207" s="14" t="s">
         <v>513</v>
-      </c>
-      <c r="F207" s="14" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="1" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="D209" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E209" s="13" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="F209" s="15" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="1" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="F211" s="14" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -13382,77 +13294,77 @@
     </row>
     <row r="213" spans="1:6">
       <c r="C213" s="13" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E213" s="13" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F213" s="21" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="B214" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C214" s="11" t="s">
         <v>424</v>
       </c>
-      <c r="B214" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C214" s="11" t="s">
-        <v>428</v>
-      </c>
       <c r="F214" s="14" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="F215" s="14" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F216" s="14" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="1" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="F217" s="14" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
     </row>
     <row r="219" spans="1:6">
       <c r="C219" s="13" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>5</v>
@@ -13461,7 +13373,7 @@
         <v>1</v>
       </c>
       <c r="F219" s="21" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -13475,7 +13387,7 @@
         <v>101</v>
       </c>
       <c r="F220" s="14" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -13489,7 +13401,7 @@
         <v>102</v>
       </c>
       <c r="F221" s="14" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -13503,7 +13415,7 @@
         <v>103</v>
       </c>
       <c r="F222" s="14" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -13517,7 +13429,7 @@
         <v>104</v>
       </c>
       <c r="F223" s="14" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -13528,10 +13440,10 @@
         <v>4</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="F224" s="14" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -13545,7 +13457,7 @@
         <v>105</v>
       </c>
       <c r="F225" s="14" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -13559,7 +13471,7 @@
         <v>106</v>
       </c>
       <c r="F226" s="14" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -13573,7 +13485,7 @@
         <v>107</v>
       </c>
       <c r="F227" s="14" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -13587,7 +13499,7 @@
         <v>108</v>
       </c>
       <c r="F228" s="14" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -13601,7 +13513,7 @@
         <v>109</v>
       </c>
       <c r="F229" s="14" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -13615,7 +13527,7 @@
         <v>110</v>
       </c>
       <c r="F230" s="14" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -13623,153 +13535,153 @@
     </row>
     <row r="232" spans="1:6">
       <c r="C232" s="24" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D232" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E232" s="13" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="F232" s="15"/>
     </row>
     <row r="233" spans="1:6">
       <c r="A233" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B233" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C233" s="10" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F233" s="14" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="234" spans="1:6">
       <c r="A234" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B234" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F234" s="14" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="235" spans="1:6">
       <c r="A235" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C235" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="B235" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C235" s="3" t="s">
-        <v>202</v>
-      </c>
       <c r="F235" s="14" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="236" spans="1:6">
       <c r="A236" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B236" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="F236" s="14" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="237" spans="1:6">
       <c r="A237" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B237" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D237" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E237" s="13" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="F237" s="15" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="238" spans="1:6">
       <c r="A238" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B238" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C238" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="B238" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="F238" s="14" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="239" spans="1:6">
       <c r="A239" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B239" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F239" s="14" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="240" spans="1:6">
       <c r="A240" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B240" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C240" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="27" thickBot="1">
-      <c r="A242" s="53" t="s">
-        <v>593</v>
-      </c>
-      <c r="B242" s="53"/>
-      <c r="C242" s="53"/>
-      <c r="D242" s="53"/>
-      <c r="E242" s="53"/>
-      <c r="F242" s="54"/>
+      <c r="A242" s="55" t="s">
+        <v>589</v>
+      </c>
+      <c r="B242" s="55"/>
+      <c r="C242" s="55"/>
+      <c r="D242" s="55"/>
+      <c r="E242" s="55"/>
+      <c r="F242" s="56"/>
     </row>
     <row r="243" spans="1:7">
       <c r="C243" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="G243" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -13777,10 +13689,10 @@
         <v>34</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G244" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -13788,10 +13700,10 @@
         <v>33</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="G245" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -13799,10 +13711,10 @@
         <v>182</v>
       </c>
       <c r="F246" s="14" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="G246" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -13810,10 +13722,10 @@
         <v>181</v>
       </c>
       <c r="F247" s="14" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="G247" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -13827,10 +13739,10 @@
         <v>28</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -13844,10 +13756,10 @@
         <v>32</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -13858,13 +13770,13 @@
         <v>4</v>
       </c>
       <c r="C251" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="F251" s="14" t="s">
         <v>568</v>
       </c>
-      <c r="F251" s="14" t="s">
-        <v>572</v>
-      </c>
       <c r="G251" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -13875,13 +13787,13 @@
         <v>4</v>
       </c>
       <c r="C252" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F252" s="14" t="s">
         <v>569</v>
       </c>
-      <c r="F252" s="14" t="s">
-        <v>573</v>
-      </c>
       <c r="G252" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -13895,61 +13807,61 @@
         <v>169</v>
       </c>
       <c r="F253" s="14" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="255" spans="1:7">
       <c r="C255" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E255" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="F255" s="22" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="G255" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C256" s="30" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="F256" s="14" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="G256" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F257" s="14" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="G257" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -13966,7 +13878,7 @@
         <v>40</v>
       </c>
       <c r="F259" s="14" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -13984,7 +13896,7 @@
         <v>75</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -14001,7 +13913,7 @@
         <v>76</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -14018,7 +13930,7 @@
         <v>142</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -14029,13 +13941,13 @@
         <v>4</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F263" s="14" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -14046,13 +13958,13 @@
         <v>4</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F264" s="14" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -14063,13 +13975,13 @@
         <v>4</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F265" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -14080,13 +13992,13 @@
         <v>4</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F266" s="14" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -14097,13 +14009,13 @@
         <v>4</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F267" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -14129,7 +14041,7 @@
         <v>145</v>
       </c>
       <c r="F273" s="14" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -14146,7 +14058,7 @@
         <v>75</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -14163,7 +14075,7 @@
         <v>76</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -14180,7 +14092,7 @@
         <v>142</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -14191,13 +14103,13 @@
         <v>4</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F277" s="14" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -14208,13 +14120,13 @@
         <v>4</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F278" s="14" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -14225,13 +14137,13 @@
         <v>4</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F279" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -14242,13 +14154,13 @@
         <v>4</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="F280" s="14" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -14259,13 +14171,13 @@
         <v>4</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F281" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -14279,7 +14191,7 @@
         <v>145</v>
       </c>
       <c r="F284" s="14" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -14293,7 +14205,7 @@
         <v>145</v>
       </c>
       <c r="F285" s="14" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -14307,7 +14219,7 @@
         <v>173</v>
       </c>
       <c r="F286" s="14" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -14321,7 +14233,7 @@
         <v>174</v>
       </c>
       <c r="F287" s="14" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -14335,7 +14247,7 @@
         <v>175</v>
       </c>
       <c r="F288" s="14" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -14352,10 +14264,10 @@
         <v>29</v>
       </c>
       <c r="F290" s="22" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -14369,10 +14281,10 @@
         <v>87</v>
       </c>
       <c r="F291" s="14" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -14386,10 +14298,10 @@
         <v>82</v>
       </c>
       <c r="F292" s="14" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -14403,10 +14315,10 @@
         <v>83</v>
       </c>
       <c r="F293" s="14" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -14420,10 +14332,10 @@
         <v>84</v>
       </c>
       <c r="F294" s="14" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -14434,13 +14346,13 @@
         <v>4</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F295" s="14" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -14451,13 +14363,13 @@
         <v>4</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="F296" s="14" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -14468,13 +14380,13 @@
         <v>4</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F297" s="14" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -14484,14 +14396,14 @@
       <c r="C302" s="2"/>
     </row>
     <row r="304" spans="1:7" ht="27" thickBot="1">
-      <c r="A304" s="53" t="s">
+      <c r="A304" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B304" s="53"/>
-      <c r="C304" s="53"/>
-      <c r="D304" s="53"/>
-      <c r="E304" s="53"/>
-      <c r="F304" s="54"/>
+      <c r="B304" s="55"/>
+      <c r="C304" s="55"/>
+      <c r="D304" s="55"/>
+      <c r="E304" s="55"/>
+      <c r="F304" s="56"/>
     </row>
     <row r="307" spans="1:6">
       <c r="C307" s="1" t="s">
@@ -14504,7 +14416,7 @@
         <v>28</v>
       </c>
       <c r="F307" s="14" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="308" spans="1:6">
@@ -14518,7 +14430,7 @@
         <v>29</v>
       </c>
       <c r="F308" s="14" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="309" spans="1:6">
@@ -14532,7 +14444,7 @@
         <v>32</v>
       </c>
       <c r="F309" s="14" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="310" spans="1:6">
@@ -14616,7 +14528,7 @@
         <v>119</v>
       </c>
       <c r="F315" s="14" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="316" spans="1:6">
@@ -14686,7 +14598,7 @@
         <v>130</v>
       </c>
       <c r="F320" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -14703,7 +14615,7 @@
         <v>75</v>
       </c>
       <c r="G321" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -14720,7 +14632,7 @@
         <v>75</v>
       </c>
       <c r="G322" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -14737,7 +14649,7 @@
         <v>76</v>
       </c>
       <c r="G323" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -14754,7 +14666,7 @@
         <v>142</v>
       </c>
       <c r="G324" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -14765,13 +14677,13 @@
         <v>4</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F325" s="14" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="G325" s="9" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -14782,13 +14694,13 @@
         <v>4</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="F326" s="14" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G326" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -14799,13 +14711,13 @@
         <v>4</v>
       </c>
       <c r="C327" s="3" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="F327" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G327" s="9" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -14816,13 +14728,13 @@
         <v>4</v>
       </c>
       <c r="C328" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F328" s="14" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G328" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -14833,13 +14745,13 @@
         <v>4</v>
       </c>
       <c r="C329" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F329" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G329" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -14853,10 +14765,10 @@
         <v>145</v>
       </c>
       <c r="F331" s="14" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -14873,7 +14785,7 @@
         <v>75</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -14890,7 +14802,7 @@
         <v>76</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -14907,7 +14819,7 @@
         <v>142</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -14918,13 +14830,13 @@
         <v>4</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="F335" s="14" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -14935,13 +14847,13 @@
         <v>4</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F336" s="14" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -14952,13 +14864,13 @@
         <v>4</v>
       </c>
       <c r="C337" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="F337" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -14969,13 +14881,13 @@
         <v>4</v>
       </c>
       <c r="C338" s="3" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F338" s="14" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -14986,13 +14898,13 @@
         <v>4</v>
       </c>
       <c r="C339" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="F339" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -15000,7 +14912,7 @@
         <v>77</v>
       </c>
       <c r="F340" s="14" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -15008,7 +14920,7 @@
         <v>78</v>
       </c>
       <c r="F341" s="14" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -15016,7 +14928,7 @@
         <v>100</v>
       </c>
       <c r="F343" s="14" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -15038,7 +14950,7 @@
         <v>99</v>
       </c>
       <c r="F347" s="14" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="348" spans="1:7">
@@ -15052,7 +14964,7 @@
         <v>43</v>
       </c>
       <c r="F348" s="14" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -15068,87 +14980,73 @@
       <c r="D349" s="9"/>
       <c r="E349" s="9"/>
       <c r="F349" s="16" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="27" thickBot="1">
-      <c r="A351" s="53" t="s">
-        <v>434</v>
-      </c>
-      <c r="B351" s="53"/>
-      <c r="C351" s="53"/>
-      <c r="D351" s="53"/>
-      <c r="E351" s="53"/>
-      <c r="F351" s="54"/>
+      <c r="A351" s="55" t="s">
+        <v>430</v>
+      </c>
+      <c r="B351" s="55"/>
+      <c r="C351" s="55"/>
+      <c r="D351" s="55"/>
+      <c r="E351" s="55"/>
+      <c r="F351" s="56"/>
     </row>
     <row r="352" spans="1:7">
       <c r="C352" s="1" t="s">
-        <v>112</v>
+        <v>657</v>
       </c>
       <c r="D352" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F352" s="14" t="s">
-        <v>114</v>
+        <v>306</v>
+      </c>
+      <c r="F352" s="22" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="353" spans="1:6">
       <c r="A353" s="1" t="s">
-        <v>113</v>
+        <v>306</v>
       </c>
       <c r="B353" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C353" s="3" t="s">
-        <v>115</v>
+        <v>659</v>
       </c>
       <c r="F353" s="14" t="s">
-        <v>116</v>
+        <v>660</v>
       </c>
     </row>
     <row r="354" spans="1:6">
       <c r="A354" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C354" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="F354" s="14" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6">
+      <c r="C356" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E356" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B354" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C354" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F354" s="14" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="355" spans="1:6">
-      <c r="A355" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B355" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C355" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F355" s="14" t="s">
-        <v>567</v>
-      </c>
-    </row>
-    <row r="356" spans="1:6">
-      <c r="A356" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B356" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C356" s="1" t="s">
-        <v>183</v>
-      </c>
       <c r="F356" s="14" t="s">
-        <v>566</v>
+        <v>114</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -15158,11 +15056,11 @@
       <c r="B357" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C357" s="1" t="s">
-        <v>194</v>
+      <c r="C357" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="F357" s="14" t="s">
-        <v>191</v>
+        <v>116</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -15173,10 +15071,10 @@
         <v>4</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>195</v>
+        <v>117</v>
       </c>
       <c r="F358" s="14" t="s">
-        <v>192</v>
+        <v>322</v>
       </c>
     </row>
     <row r="359" spans="1:6">
@@ -15187,52 +15085,52 @@
         <v>4</v>
       </c>
       <c r="C359" s="1" t="s">
-        <v>605</v>
+        <v>184</v>
       </c>
       <c r="F359" s="14" t="s">
-        <v>606</v>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6">
+      <c r="A360" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B360" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F360" s="14" t="s">
+        <v>562</v>
       </c>
     </row>
     <row r="361" spans="1:6">
-      <c r="C361" s="1" t="s">
+      <c r="A361" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B361" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C361" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="F361" s="14" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6">
+      <c r="C363" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D361" s="1" t="s">
+      <c r="D363" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E361" s="1" t="s">
+      <c r="E363" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F361" s="14" t="s">
+      <c r="F363" s="14" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6">
-      <c r="A362" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B362" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C362" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F362" s="14" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6">
-      <c r="A363" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B363" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C363" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="F363" s="14" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="364" spans="1:6">
@@ -15243,10 +15141,10 @@
         <v>4</v>
       </c>
       <c r="C364" s="2" t="s">
-        <v>212</v>
+        <v>150</v>
       </c>
       <c r="F364" s="14" t="s">
-        <v>321</v>
+        <v>127</v>
       </c>
     </row>
     <row r="365" spans="1:6">
@@ -15256,11 +15154,11 @@
       <c r="B365" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C365" s="3" t="s">
-        <v>217</v>
+      <c r="C365" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="F365" s="14" t="s">
-        <v>219</v>
+        <v>316</v>
       </c>
     </row>
     <row r="366" spans="1:6">
@@ -15270,11 +15168,11 @@
       <c r="B366" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C366" s="3" t="s">
-        <v>218</v>
+      <c r="C366" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="F366" s="14" t="s">
-        <v>219</v>
+        <v>317</v>
       </c>
     </row>
     <row r="367" spans="1:6">
@@ -15285,10 +15183,10 @@
         <v>4</v>
       </c>
       <c r="C367" s="3" t="s">
-        <v>152</v>
+        <v>213</v>
       </c>
       <c r="F367" s="14" t="s">
-        <v>128</v>
+        <v>215</v>
       </c>
     </row>
     <row r="368" spans="1:6">
@@ -15299,10 +15197,10 @@
         <v>4</v>
       </c>
       <c r="C368" s="3" t="s">
-        <v>151</v>
+        <v>214</v>
       </c>
       <c r="F368" s="14" t="s">
-        <v>129</v>
+        <v>215</v>
       </c>
     </row>
     <row r="369" spans="1:6">
@@ -15313,10 +15211,10 @@
         <v>4</v>
       </c>
       <c r="C369" s="3" t="s">
-        <v>185</v>
+        <v>152</v>
       </c>
       <c r="F369" s="14" t="s">
-        <v>186</v>
+        <v>128</v>
       </c>
     </row>
     <row r="370" spans="1:6">
@@ -15327,10 +15225,10 @@
         <v>4</v>
       </c>
       <c r="C370" s="3" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="F370" s="14" t="s">
-        <v>189</v>
+        <v>129</v>
       </c>
     </row>
     <row r="371" spans="1:6">
@@ -15341,10 +15239,10 @@
         <v>4</v>
       </c>
       <c r="C371" s="3" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="F371" s="14" t="s">
-        <v>154</v>
+        <v>186</v>
       </c>
     </row>
     <row r="372" spans="1:6">
@@ -15355,9 +15253,37 @@
         <v>4</v>
       </c>
       <c r="C372" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F372" s="14" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6">
+      <c r="A373" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B373" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C373" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F373" s="14" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6">
+      <c r="A374" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B374" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C374" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="F372" s="14" t="s">
+      <c r="F374" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -15366,7 +15292,7 @@
         <v>126</v>
       </c>
       <c r="F377" s="14" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="378" spans="1:6">
@@ -15390,7 +15316,7 @@
         <v>131</v>
       </c>
       <c r="F380" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="381" spans="1:6">
@@ -15417,15 +15343,15 @@
         <v>136</v>
       </c>
       <c r="F385" s="14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="386" spans="1:6">
       <c r="C386" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F386" s="14" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="387" spans="1:6">
@@ -15433,15 +15359,15 @@
         <v>187</v>
       </c>
       <c r="F387" s="14" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="388" spans="1:6">
       <c r="C388" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F388" s="14" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="389" spans="1:6">
@@ -15452,7 +15378,7 @@
         <v>5</v>
       </c>
       <c r="E389" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F389" s="14" t="s">
         <v>138</v>
@@ -15460,7 +15386,7 @@
     </row>
     <row r="390" spans="1:6">
       <c r="A390" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>4</v>
@@ -15474,203 +15400,203 @@
     </row>
     <row r="391" spans="1:6">
       <c r="A391" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B391" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C391" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="F391" s="14" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="392" spans="1:6">
       <c r="A392" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C392" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F392" s="14" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="393" spans="1:6">
       <c r="A393" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B393" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C393" s="3" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F393" s="14" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="396" spans="1:6" ht="27" thickBot="1">
-      <c r="A396" s="53" t="s">
-        <v>262</v>
-      </c>
-      <c r="B396" s="53"/>
-      <c r="C396" s="53"/>
-      <c r="D396" s="53"/>
-      <c r="E396" s="53"/>
-      <c r="F396" s="54"/>
+      <c r="A396" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="B396" s="55"/>
+      <c r="C396" s="55"/>
+      <c r="D396" s="55"/>
+      <c r="E396" s="55"/>
+      <c r="F396" s="56"/>
     </row>
     <row r="397" spans="1:6">
       <c r="C397" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D397" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E397" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F397" s="14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="398" spans="1:6">
       <c r="C398" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="F398" s="14" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="399" spans="1:6">
       <c r="C399" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="F399" s="14" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="400" spans="1:6">
       <c r="C400" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="F400" s="14" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="401" spans="3:6">
       <c r="C401" s="1" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F401" s="14" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="402" spans="3:6">
       <c r="C402" s="1" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="F402" s="14" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="403" spans="3:6">
       <c r="C403" s="1" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F403" s="14" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="404" spans="3:6">
       <c r="C404" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="F404" s="14" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="405" spans="3:6">
       <c r="C405" s="1" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F405" s="14" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="406" spans="3:6">
       <c r="C406" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="F406" s="14" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="407" spans="3:6">
       <c r="C407" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="F407" s="14" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="409" spans="3:6">
       <c r="C409" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F409" s="14" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="410" spans="3:6">
       <c r="C410" s="1" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F410" s="14" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="411" spans="3:6">
       <c r="C411" s="1" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="F411" s="14" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="412" spans="3:6">
       <c r="C412" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F412" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="414" spans="3:6">
       <c r="C414" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="417" spans="1:6" ht="27" thickBot="1">
-      <c r="A417" s="53" t="s">
-        <v>271</v>
-      </c>
-      <c r="B417" s="53"/>
-      <c r="C417" s="53"/>
-      <c r="D417" s="53"/>
-      <c r="E417" s="53"/>
-      <c r="F417" s="54"/>
+      <c r="A417" s="55" t="s">
+        <v>267</v>
+      </c>
+      <c r="B417" s="55"/>
+      <c r="C417" s="55"/>
+      <c r="D417" s="55"/>
+      <c r="E417" s="55"/>
+      <c r="F417" s="56"/>
     </row>
     <row r="418" spans="1:6">
       <c r="C418" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="F418" s="14" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="419" spans="1:6">
@@ -15681,7 +15607,7 @@
     </row>
     <row r="420" spans="1:6">
       <c r="C420" s="13" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D420" s="13" t="s">
         <v>5</v>
@@ -15690,7 +15616,7 @@
         <v>23</v>
       </c>
       <c r="F420" s="21" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -15704,12 +15630,12 @@
         <v>71</v>
       </c>
       <c r="F421" s="14" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="423" spans="1:6">
       <c r="C423" s="13" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D423" s="13" t="s">
         <v>5</v>
@@ -15718,7 +15644,7 @@
         <v>29</v>
       </c>
       <c r="F423" s="15" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="424" spans="1:6">
@@ -15729,38 +15655,38 @@
         <v>4</v>
       </c>
       <c r="C424" s="8" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F424" s="14" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
     </row>
     <row r="426" spans="1:6">
       <c r="C426" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D426" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E426" s="1" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F426" s="22" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="427" spans="1:6">
       <c r="C427" s="13" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="D427" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E427" s="13" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F427" s="21" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="428" spans="1:6">
@@ -15771,10 +15697,10 @@
         <v>4</v>
       </c>
       <c r="C428" s="10" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="F428" s="14" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="429" spans="1:6">
@@ -15785,10 +15711,10 @@
         <v>4</v>
       </c>
       <c r="C429" s="2" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="F429" s="14" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="430" spans="1:6">
@@ -15799,10 +15725,10 @@
         <v>4</v>
       </c>
       <c r="C430" s="12" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="F430" s="14" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -15813,10 +15739,10 @@
         <v>4</v>
       </c>
       <c r="C431" s="12" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F431" s="14" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
     </row>
     <row r="432" spans="1:6">
@@ -15827,10 +15753,10 @@
         <v>4</v>
       </c>
       <c r="C432" s="12" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="F432" s="14" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -15841,10 +15767,10 @@
         <v>4</v>
       </c>
       <c r="C433" s="8" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="F433" s="14" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -15855,10 +15781,10 @@
         <v>4</v>
       </c>
       <c r="C434" s="8" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="F434" s="14" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -15869,10 +15795,10 @@
         <v>4</v>
       </c>
       <c r="C435" s="8" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F435" s="14" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -15883,10 +15809,10 @@
         <v>4</v>
       </c>
       <c r="C436" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="F436" s="14" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="437" spans="1:7">
@@ -15900,52 +15826,52 @@
         <v>5</v>
       </c>
       <c r="E438" s="13" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="F438" s="21" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
     </row>
     <row r="439" spans="1:7">
       <c r="A439" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F439" s="14" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="440" spans="1:7">
       <c r="A440" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C440" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F440" s="14" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="441" spans="1:7">
       <c r="A441" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B441" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C441" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="F441" s="14" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="443" spans="1:7">
@@ -15962,6 +15888,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A417:F417"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A396:F396"/>
     <mergeCell ref="A351:F351"/>
@@ -15969,12 +15901,6 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
-    <mergeCell ref="A417:F417"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds the word 'add' to the 'interactive staging' command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B9C173-404C-194F-8BC1-7800521D7E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82142844-792C-EF47-8851-13CDB0FDFC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26180" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
@@ -3057,28 +3057,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">git (-i </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --interactive)</t>
-    </r>
-  </si>
-  <si>
     <t>[i]</t>
   </si>
   <si>
@@ -10295,6 +10273,28 @@
         <rFont val="Menlo Regular"/>
       </rPr>
       <t>option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git add (-i </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> --interactive)</t>
     </r>
   </si>
 </sst>
@@ -10749,12 +10749,12 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11075,8 +11075,8 @@
   </sheetPr>
   <dimension ref="A1:G445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A342" zoomScale="168" zoomScaleNormal="168" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="A361" sqref="A361:XFD366"/>
+    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="168" zoomScaleNormal="168" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C397" sqref="C397"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11091,83 +11091,83 @@
   <sheetData>
     <row r="1" spans="1:6" ht="31">
       <c r="A1" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="18" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="19" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -11175,25 +11175,25 @@
         <v>44</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -11202,12 +11202,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -11216,12 +11216,12 @@
         <v>2</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="13" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>5</v>
@@ -11230,7 +11230,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -11241,12 +11241,12 @@
         <v>4</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="32" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -11260,7 +11260,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -11274,7 +11274,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -11285,10 +11285,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>486</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -11299,10 +11299,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>652</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -11313,10 +11313,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>488</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>489</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -11330,7 +11330,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -11344,7 +11344,7 @@
         <v>191</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -11355,10 +11355,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -11372,7 +11372,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -11386,7 +11386,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -11400,29 +11400,29 @@
         <v>53</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="C29" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>600</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="33" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -11434,16 +11434,16 @@
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="21" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="33"/>
       <c r="C33" s="35" t="s">
+        <v>605</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>606</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -11453,7 +11453,7 @@
     <row r="35" spans="1:6" ht="20" thickBot="1">
       <c r="A35" s="33"/>
       <c r="C35" s="36" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
@@ -11465,25 +11465,25 @@
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="21" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="33"/>
       <c r="C37" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>610</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="33"/>
       <c r="C38" s="39" t="s">
+        <v>611</v>
+      </c>
+      <c r="F38" s="14" t="s">
         <v>612</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>613</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -11497,43 +11497,43 @@
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="21" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="33"/>
       <c r="C41" s="41" t="s">
+        <v>614</v>
+      </c>
+      <c r="F41" s="14" t="s">
         <v>615</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="33"/>
       <c r="C42" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="F42" s="14" t="s">
         <v>617</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="33"/>
       <c r="C43" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="F43" s="14" t="s">
         <v>619</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="40">
       <c r="A44" s="33"/>
       <c r="C44" s="39" t="s">
+        <v>620</v>
+      </c>
+      <c r="F44" s="42" t="s">
         <v>621</v>
-      </c>
-      <c r="F44" s="42" t="s">
-        <v>622</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -11543,10 +11543,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="33"/>
-      <c r="C46" s="55" t="s">
-        <v>623</v>
-      </c>
-      <c r="D46" s="56"/>
+      <c r="C46" s="57" t="s">
+        <v>622</v>
+      </c>
+      <c r="D46" s="58"/>
       <c r="E46" s="37"/>
       <c r="F46" s="43"/>
     </row>
@@ -11556,52 +11556,52 @@
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="46" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="33"/>
       <c r="C48" s="41" t="s">
+        <v>614</v>
+      </c>
+      <c r="F48" s="14" t="s">
         <v>615</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="33"/>
       <c r="C49" s="4" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="33"/>
       <c r="C50" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="F50" s="14" t="s">
         <v>626</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="40">
       <c r="A51" s="33"/>
       <c r="C51" s="39" t="s">
+        <v>627</v>
+      </c>
+      <c r="F51" s="42" t="s">
         <v>628</v>
-      </c>
-      <c r="F51" s="42" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="40">
       <c r="A52" s="33"/>
       <c r="C52" s="39" t="s">
+        <v>629</v>
+      </c>
+      <c r="F52" s="42" t="s">
         <v>630</v>
-      </c>
-      <c r="F52" s="42" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -11612,7 +11612,7 @@
     <row r="54" spans="1:6" ht="20" thickBot="1">
       <c r="A54" s="33"/>
       <c r="C54" s="36" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D54" s="37"/>
       <c r="E54" s="37"/>
@@ -11624,52 +11624,52 @@
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="21" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="27">
       <c r="A56" s="33"/>
       <c r="C56" s="51" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F56" s="47" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="33"/>
       <c r="C57" s="39" t="s">
+        <v>633</v>
+      </c>
+      <c r="F57" s="42" t="s">
         <v>634</v>
-      </c>
-      <c r="F57" s="42" t="s">
-        <v>635</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="33"/>
       <c r="C58" s="39" t="s">
+        <v>635</v>
+      </c>
+      <c r="F58" s="42" t="s">
         <v>636</v>
-      </c>
-      <c r="F58" s="42" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="26">
       <c r="A59" s="33"/>
       <c r="C59" s="50" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F59" s="49" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="40">
       <c r="A60" s="33"/>
       <c r="C60" s="41" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F60" s="47" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -11683,25 +11683,25 @@
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="21" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="27">
       <c r="A63" s="33"/>
       <c r="C63" s="48" t="s">
+        <v>642</v>
+      </c>
+      <c r="F63" s="47" t="s">
         <v>643</v>
-      </c>
-      <c r="F63" s="47" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="26">
       <c r="A64" s="33"/>
       <c r="C64" s="50" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -11715,25 +11715,25 @@
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="21" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="27">
       <c r="A67" s="33"/>
       <c r="C67" s="52" t="s">
+        <v>648</v>
+      </c>
+      <c r="F67" s="47" t="s">
         <v>649</v>
-      </c>
-      <c r="F67" s="47" t="s">
-        <v>650</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26">
       <c r="A68" s="33"/>
       <c r="C68" s="50" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -11742,21 +11742,21 @@
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="54"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="56"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -11764,15 +11764,15 @@
         <v>155</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="C73" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -11780,7 +11780,7 @@
         <v>154</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -11788,7 +11788,7 @@
         <v>10</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -11796,7 +11796,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -11804,7 +11804,7 @@
         <v>12</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -11812,7 +11812,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -11820,15 +11820,15 @@
         <v>109</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17">
       <c r="C80" s="9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -11836,15 +11836,15 @@
         <v>51</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="C82" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -11852,7 +11852,7 @@
         <v>65</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -11860,7 +11860,7 @@
         <v>156</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -11868,28 +11868,28 @@
         <v>157</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="53" t="s">
+      <c r="A87" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="53"/>
-      <c r="C87" s="53"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="54"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="56"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -11897,7 +11897,7 @@
         <v>18</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -11905,39 +11905,39 @@
         <v>19</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="C91" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="C92" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="C93" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="C94" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -11945,7 +11945,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -11953,25 +11953,25 @@
         <v>25</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="53" t="s">
+      <c r="A98" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="53"/>
-      <c r="C98" s="53"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="53"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="55"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F99" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -11979,7 +11979,7 @@
         <v>33</v>
       </c>
       <c r="F100" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -11987,7 +11987,7 @@
         <v>181</v>
       </c>
       <c r="F101" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -11995,7 +11995,7 @@
         <v>180</v>
       </c>
       <c r="F102" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -12003,7 +12003,7 @@
         <v>22</v>
       </c>
       <c r="F103" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -12011,7 +12011,7 @@
         <v>98</v>
       </c>
       <c r="F104" s="14" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -12019,7 +12019,7 @@
         <v>96</v>
       </c>
       <c r="F105" s="14" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -12027,15 +12027,15 @@
         <v>97</v>
       </c>
       <c r="F106" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="C107" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F107" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -12043,7 +12043,7 @@
         <v>24</v>
       </c>
       <c r="F108" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -12051,7 +12051,7 @@
         <v>206</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -12059,7 +12059,7 @@
         <v>207</v>
       </c>
       <c r="F110" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -12067,7 +12067,7 @@
         <v>208</v>
       </c>
       <c r="F111" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -12075,7 +12075,7 @@
         <v>65</v>
       </c>
       <c r="F112" s="14" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -12083,7 +12083,7 @@
         <v>156</v>
       </c>
       <c r="F113" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -12091,26 +12091,26 @@
         <v>157</v>
       </c>
       <c r="F114" s="14" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="C116" s="13" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D116" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>4</v>
@@ -12119,12 +12119,12 @@
         <v>161</v>
       </c>
       <c r="F117" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>4</v>
@@ -12133,12 +12133,12 @@
         <v>166</v>
       </c>
       <c r="F118" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>4</v>
@@ -12147,12 +12147,12 @@
         <v>167</v>
       </c>
       <c r="F119" s="14" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>4</v>
@@ -12161,40 +12161,40 @@
         <v>160</v>
       </c>
       <c r="F120" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F121" s="14" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F122" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D124" s="13" t="s">
         <v>5</v>
@@ -12203,7 +12203,7 @@
         <v>26</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -12217,7 +12217,7 @@
         <v>64</v>
       </c>
       <c r="F125" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -12228,10 +12228,10 @@
         <v>4</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="F126" s="14" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -12245,7 +12245,7 @@
         <v>63</v>
       </c>
       <c r="F127" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -12256,10 +12256,10 @@
         <v>4</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F128" s="14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -12273,7 +12273,7 @@
         <v>158</v>
       </c>
       <c r="F129" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -12284,36 +12284,36 @@
         <v>4</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F130" s="14" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="131" spans="1:6">
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="53" t="s">
+      <c r="A132" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="53"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="53"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="54"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="55"/>
+      <c r="E132" s="55"/>
+      <c r="F132" s="56"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F133" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D135" s="13" t="s">
         <v>5</v>
@@ -12322,7 +12322,7 @@
         <v>23</v>
       </c>
       <c r="F135" s="15" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -12333,10 +12333,10 @@
         <v>4</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F136" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -12350,7 +12350,7 @@
         <v>184</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -12364,7 +12364,7 @@
         <v>67</v>
       </c>
       <c r="F138" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -12378,7 +12378,7 @@
         <v>70</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -12392,7 +12392,7 @@
         <v>68</v>
       </c>
       <c r="F140" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -12411,7 +12411,7 @@
         <v>71</v>
       </c>
       <c r="F142" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="143" spans="1:6">
@@ -12425,7 +12425,7 @@
         <v>62</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -12439,7 +12439,7 @@
         <v>60</v>
       </c>
       <c r="F144" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -12453,7 +12453,7 @@
         <v>61</v>
       </c>
       <c r="F145" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -12464,10 +12464,10 @@
         <v>4</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="F146" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -12481,7 +12481,7 @@
         <v>59</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -12495,7 +12495,7 @@
         <v>58</v>
       </c>
       <c r="F148" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -12509,7 +12509,7 @@
         <v>57</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -12523,7 +12523,7 @@
         <v>56</v>
       </c>
       <c r="F150" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -12537,7 +12537,7 @@
         <v>27</v>
       </c>
       <c r="F151" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="152" spans="1:6">
@@ -12551,7 +12551,7 @@
         <v>66</v>
       </c>
       <c r="F152" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -12562,10 +12562,10 @@
         <v>4</v>
       </c>
       <c r="C153" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F153" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -12579,7 +12579,7 @@
         <v>1</v>
       </c>
       <c r="F155" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -12593,7 +12593,7 @@
         <v>1</v>
       </c>
       <c r="F156" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -12607,7 +12607,7 @@
         <v>38</v>
       </c>
       <c r="F157" s="14" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -12621,7 +12621,7 @@
         <v>1</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -12635,7 +12635,7 @@
         <v>39</v>
       </c>
       <c r="F159" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -12649,7 +12649,7 @@
         <v>40</v>
       </c>
       <c r="F160" s="15" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -12663,7 +12663,7 @@
         <v>85</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -12677,7 +12677,7 @@
         <v>87</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -12688,10 +12688,10 @@
         <v>4</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -12705,7 +12705,7 @@
         <v>88</v>
       </c>
       <c r="F164" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -12719,7 +12719,7 @@
         <v>89</v>
       </c>
       <c r="F165" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -12730,10 +12730,10 @@
         <v>4</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -12747,7 +12747,7 @@
         <v>90</v>
       </c>
       <c r="F167" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -12761,7 +12761,7 @@
         <v>91</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -12772,10 +12772,10 @@
         <v>4</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F169" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -12789,7 +12789,7 @@
         <v>92</v>
       </c>
       <c r="F170" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -12803,7 +12803,7 @@
         <v>93</v>
       </c>
       <c r="F171" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -12817,7 +12817,7 @@
         <v>94</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -12831,7 +12831,7 @@
         <v>95</v>
       </c>
       <c r="F173" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -12842,10 +12842,10 @@
         <v>4</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F174" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -12856,10 +12856,10 @@
         <v>4</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F175" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -12873,7 +12873,7 @@
         <v>200</v>
       </c>
       <c r="F176" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -12887,7 +12887,7 @@
         <v>201</v>
       </c>
       <c r="F177" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -12901,96 +12901,96 @@
         <v>202</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="180" spans="1:6">
       <c r="C180" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D180" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E180" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="F180" s="21" t="s">
         <v>418</v>
-      </c>
-      <c r="F180" s="21" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F181" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F182" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C183" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F183" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C184" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F184" s="14" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="186" spans="1:6">
       <c r="C186" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F186" s="22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="187" spans="1:6">
       <c r="C187" s="26" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D187" s="25" t="s">
         <v>5</v>
@@ -12999,21 +12999,21 @@
         <v>73</v>
       </c>
       <c r="F187" s="27" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="188" spans="1:6">
       <c r="C188" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E188" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -13024,10 +13024,10 @@
         <v>4</v>
       </c>
       <c r="C189" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F189" s="14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -13038,10 +13038,10 @@
         <v>4</v>
       </c>
       <c r="C190" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F190" s="14" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -13052,10 +13052,10 @@
         <v>4</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="F191" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -13066,10 +13066,10 @@
         <v>4</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -13080,10 +13080,10 @@
         <v>4</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F193" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -13094,31 +13094,31 @@
         <v>4</v>
       </c>
       <c r="C194" s="5" t="s">
+        <v>497</v>
+      </c>
+      <c r="F194" s="14" t="s">
         <v>498</v>
-      </c>
-      <c r="F194" s="14" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="53" t="s">
-        <v>426</v>
-      </c>
-      <c r="B196" s="53"/>
-      <c r="C196" s="53"/>
-      <c r="D196" s="53"/>
-      <c r="E196" s="53"/>
-      <c r="F196" s="53"/>
+      <c r="A196" s="55" t="s">
+        <v>425</v>
+      </c>
+      <c r="B196" s="55"/>
+      <c r="C196" s="55"/>
+      <c r="D196" s="55"/>
+      <c r="E196" s="55"/>
+      <c r="F196" s="55"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F197" s="28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -13135,7 +13135,7 @@
         <v>37</v>
       </c>
       <c r="F199" s="21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -13146,10 +13146,10 @@
         <v>4</v>
       </c>
       <c r="C200" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F200" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -13160,10 +13160,10 @@
         <v>4</v>
       </c>
       <c r="C201" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F201" s="14" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -13171,164 +13171,164 @@
     </row>
     <row r="203" spans="1:6">
       <c r="C203" s="24" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D203" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E203" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F203" s="21" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="204" spans="1:6">
       <c r="A204" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C204" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D204" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F204" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="205" spans="1:6">
       <c r="A205" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C205" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D205" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F205" s="14" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="206" spans="1:6">
       <c r="A206" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C206" s="11" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D206" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F206" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="207" spans="1:6">
       <c r="A207" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F207" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="208" spans="1:6">
       <c r="A208" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C208" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D208" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="209" spans="1:6">
       <c r="A209" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D209" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E209" s="13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F209" s="15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F211" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -13336,77 +13336,77 @@
     </row>
     <row r="213" spans="1:6">
       <c r="C213" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E213" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="F213" s="21" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F214" s="14" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F215" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C216" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F216" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F217" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="219" spans="1:6">
       <c r="C219" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D219" s="13" t="s">
         <v>5</v>
@@ -13415,7 +13415,7 @@
         <v>1</v>
       </c>
       <c r="F219" s="21" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -13429,7 +13429,7 @@
         <v>101</v>
       </c>
       <c r="F220" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -13443,7 +13443,7 @@
         <v>102</v>
       </c>
       <c r="F221" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -13457,7 +13457,7 @@
         <v>103</v>
       </c>
       <c r="F222" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="223" spans="1:6">
@@ -13471,7 +13471,7 @@
         <v>104</v>
       </c>
       <c r="F223" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="224" spans="1:6">
@@ -13482,10 +13482,10 @@
         <v>4</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F224" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="225" spans="1:6">
@@ -13499,7 +13499,7 @@
         <v>105</v>
       </c>
       <c r="F225" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -13513,7 +13513,7 @@
         <v>106</v>
       </c>
       <c r="F226" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -13527,7 +13527,7 @@
         <v>107</v>
       </c>
       <c r="F227" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -13541,7 +13541,7 @@
         <v>108</v>
       </c>
       <c r="F228" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -13555,7 +13555,7 @@
         <v>109</v>
       </c>
       <c r="F229" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -13569,7 +13569,7 @@
         <v>110</v>
       </c>
       <c r="F230" s="14" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -13577,7 +13577,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="C232" s="24" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D232" s="13" t="s">
         <v>5</v>
@@ -13598,7 +13598,7 @@
         <v>194</v>
       </c>
       <c r="F233" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -13612,7 +13612,7 @@
         <v>196</v>
       </c>
       <c r="F234" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -13626,7 +13626,7 @@
         <v>195</v>
       </c>
       <c r="F235" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -13640,7 +13640,7 @@
         <v>203</v>
       </c>
       <c r="F236" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -13651,7 +13651,7 @@
         <v>4</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D237" s="13" t="s">
         <v>5</v>
@@ -13660,7 +13660,7 @@
         <v>193</v>
       </c>
       <c r="F237" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -13674,7 +13674,7 @@
         <v>197</v>
       </c>
       <c r="F238" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -13688,7 +13688,7 @@
         <v>198</v>
       </c>
       <c r="F239" s="14" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -13702,28 +13702,28 @@
         <v>199</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="27" thickBot="1">
-      <c r="A242" s="53" t="s">
-        <v>586</v>
-      </c>
-      <c r="B242" s="53"/>
-      <c r="C242" s="53"/>
-      <c r="D242" s="53"/>
-      <c r="E242" s="53"/>
-      <c r="F242" s="54"/>
+      <c r="A242" s="55" t="s">
+        <v>585</v>
+      </c>
+      <c r="B242" s="55"/>
+      <c r="C242" s="55"/>
+      <c r="D242" s="55"/>
+      <c r="E242" s="55"/>
+      <c r="F242" s="56"/>
     </row>
     <row r="243" spans="1:7">
       <c r="C243" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="G243" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -13731,10 +13731,10 @@
         <v>34</v>
       </c>
       <c r="F244" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G244" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -13742,10 +13742,10 @@
         <v>33</v>
       </c>
       <c r="F245" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="G245" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -13753,10 +13753,10 @@
         <v>181</v>
       </c>
       <c r="F246" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G246" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -13764,10 +13764,10 @@
         <v>180</v>
       </c>
       <c r="F247" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G247" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -13781,10 +13781,10 @@
         <v>28</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -13798,10 +13798,10 @@
         <v>32</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -13812,13 +13812,13 @@
         <v>4</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -13829,13 +13829,13 @@
         <v>4</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F252" s="14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -13849,61 +13849,61 @@
         <v>168</v>
       </c>
       <c r="F253" s="14" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="255" spans="1:7">
       <c r="C255" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E255" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="F255" s="22" t="s">
+        <v>549</v>
+      </c>
+      <c r="G255" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="F255" s="22" t="s">
-        <v>550</v>
-      </c>
-      <c r="G255" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256" s="30" t="s">
+        <v>548</v>
+      </c>
+      <c r="F256" s="14" t="s">
+        <v>575</v>
+      </c>
+      <c r="G256" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C256" s="30" t="s">
-        <v>549</v>
-      </c>
-      <c r="F256" s="14" t="s">
-        <v>576</v>
-      </c>
-      <c r="G256" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="F257" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="G257" s="1" t="s">
         <v>547</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>553</v>
-      </c>
-      <c r="F257" s="14" t="s">
-        <v>585</v>
-      </c>
-      <c r="G257" s="1" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -13920,7 +13920,7 @@
         <v>40</v>
       </c>
       <c r="F259" s="14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -13938,7 +13938,7 @@
         <v>75</v>
       </c>
       <c r="G260" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="261" spans="1:7">
@@ -13955,7 +13955,7 @@
         <v>76</v>
       </c>
       <c r="G261" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="262" spans="1:7">
@@ -13972,7 +13972,7 @@
         <v>141</v>
       </c>
       <c r="G262" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="263" spans="1:7">
@@ -13983,13 +13983,13 @@
         <v>4</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F263" s="14" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -14000,13 +14000,13 @@
         <v>4</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F264" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -14020,10 +14020,10 @@
         <v>214</v>
       </c>
       <c r="F265" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -14034,13 +14034,13 @@
         <v>4</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F266" s="14" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -14051,13 +14051,13 @@
         <v>4</v>
       </c>
       <c r="C267" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F267" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F267" s="14" t="s">
-        <v>244</v>
-      </c>
       <c r="G267" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -14083,7 +14083,7 @@
         <v>144</v>
       </c>
       <c r="F273" s="14" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -14100,7 +14100,7 @@
         <v>75</v>
       </c>
       <c r="G274" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="275" spans="1:7">
@@ -14117,7 +14117,7 @@
         <v>76</v>
       </c>
       <c r="G275" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" spans="1:7">
@@ -14134,7 +14134,7 @@
         <v>141</v>
       </c>
       <c r="G276" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="277" spans="1:7">
@@ -14145,13 +14145,13 @@
         <v>4</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F277" s="14" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -14162,13 +14162,13 @@
         <v>4</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F278" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -14182,10 +14182,10 @@
         <v>215</v>
       </c>
       <c r="F279" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -14196,13 +14196,13 @@
         <v>4</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F280" s="14" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -14213,13 +14213,13 @@
         <v>4</v>
       </c>
       <c r="C281" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F281" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F281" s="14" t="s">
-        <v>244</v>
-      </c>
       <c r="G281" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -14233,7 +14233,7 @@
         <v>144</v>
       </c>
       <c r="F284" s="14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -14247,7 +14247,7 @@
         <v>144</v>
       </c>
       <c r="F285" s="14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -14261,7 +14261,7 @@
         <v>172</v>
       </c>
       <c r="F286" s="14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -14275,7 +14275,7 @@
         <v>173</v>
       </c>
       <c r="F287" s="14" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -14289,7 +14289,7 @@
         <v>174</v>
       </c>
       <c r="F288" s="14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -14306,10 +14306,10 @@
         <v>29</v>
       </c>
       <c r="F290" s="22" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -14323,10 +14323,10 @@
         <v>87</v>
       </c>
       <c r="F291" s="14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -14340,10 +14340,10 @@
         <v>82</v>
       </c>
       <c r="F292" s="14" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -14357,10 +14357,10 @@
         <v>83</v>
       </c>
       <c r="F293" s="14" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -14374,10 +14374,10 @@
         <v>84</v>
       </c>
       <c r="F294" s="14" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -14388,13 +14388,13 @@
         <v>4</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F295" s="14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -14405,13 +14405,13 @@
         <v>4</v>
       </c>
       <c r="C296" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="F296" s="14" t="s">
         <v>588</v>
       </c>
-      <c r="F296" s="14" t="s">
-        <v>589</v>
-      </c>
       <c r="G296" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -14422,13 +14422,13 @@
         <v>4</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F297" s="14" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -14438,14 +14438,14 @@
       <c r="C302" s="2"/>
     </row>
     <row r="304" spans="1:7" ht="27" thickBot="1">
-      <c r="A304" s="53" t="s">
+      <c r="A304" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B304" s="53"/>
-      <c r="C304" s="53"/>
-      <c r="D304" s="53"/>
-      <c r="E304" s="53"/>
-      <c r="F304" s="54"/>
+      <c r="B304" s="55"/>
+      <c r="C304" s="55"/>
+      <c r="D304" s="55"/>
+      <c r="E304" s="55"/>
+      <c r="F304" s="56"/>
     </row>
     <row r="307" spans="1:6">
       <c r="C307" s="1" t="s">
@@ -14458,7 +14458,7 @@
         <v>28</v>
       </c>
       <c r="F307" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="308" spans="1:6">
@@ -14472,7 +14472,7 @@
         <v>29</v>
       </c>
       <c r="F308" s="14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="309" spans="1:6">
@@ -14486,7 +14486,7 @@
         <v>32</v>
       </c>
       <c r="F309" s="14" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="310" spans="1:6">
@@ -14570,7 +14570,7 @@
         <v>118</v>
       </c>
       <c r="F315" s="14" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="316" spans="1:6">
@@ -14640,7 +14640,7 @@
         <v>129</v>
       </c>
       <c r="F320" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="321" spans="1:7">
@@ -14657,7 +14657,7 @@
         <v>75</v>
       </c>
       <c r="G321" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -14674,7 +14674,7 @@
         <v>75</v>
       </c>
       <c r="G322" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -14691,7 +14691,7 @@
         <v>76</v>
       </c>
       <c r="G323" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -14708,7 +14708,7 @@
         <v>141</v>
       </c>
       <c r="G324" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -14719,13 +14719,13 @@
         <v>4</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F325" s="14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G325" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -14736,13 +14736,13 @@
         <v>4</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F326" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G326" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="327" spans="1:7">
@@ -14756,10 +14756,10 @@
         <v>214</v>
       </c>
       <c r="F327" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G327" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -14773,10 +14773,10 @@
         <v>213</v>
       </c>
       <c r="F328" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G328" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="329" spans="1:7">
@@ -14787,13 +14787,13 @@
         <v>4</v>
       </c>
       <c r="C329" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F329" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F329" s="14" t="s">
-        <v>244</v>
-      </c>
       <c r="G329" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="331" spans="1:7">
@@ -14807,10 +14807,10 @@
         <v>144</v>
       </c>
       <c r="F331" s="14" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -14827,7 +14827,7 @@
         <v>75</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -14844,7 +14844,7 @@
         <v>76</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -14861,7 +14861,7 @@
         <v>141</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -14872,13 +14872,13 @@
         <v>4</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F335" s="14" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -14889,13 +14889,13 @@
         <v>4</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F336" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="337" spans="1:7">
@@ -14909,10 +14909,10 @@
         <v>215</v>
       </c>
       <c r="F337" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -14926,10 +14926,10 @@
         <v>213</v>
       </c>
       <c r="F338" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="339" spans="1:7">
@@ -14940,13 +14940,13 @@
         <v>4</v>
       </c>
       <c r="C339" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="F339" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="F339" s="14" t="s">
-        <v>244</v>
-      </c>
       <c r="G339" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="340" spans="1:7">
@@ -14954,7 +14954,7 @@
         <v>77</v>
       </c>
       <c r="F340" s="14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -14962,7 +14962,7 @@
         <v>78</v>
       </c>
       <c r="F341" s="14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -14970,7 +14970,7 @@
         <v>100</v>
       </c>
       <c r="F343" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="346" spans="1:7">
@@ -14992,7 +14992,7 @@
         <v>99</v>
       </c>
       <c r="F347" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="348" spans="1:7">
@@ -15006,7 +15006,7 @@
         <v>43</v>
       </c>
       <c r="F348" s="14" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="349" spans="1:7">
@@ -15022,22 +15022,22 @@
       <c r="D349" s="9"/>
       <c r="E349" s="9"/>
       <c r="F349" s="16" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="351" spans="1:7" ht="27" thickBot="1">
-      <c r="A351" s="53" t="s">
-        <v>427</v>
-      </c>
-      <c r="B351" s="53"/>
-      <c r="C351" s="53"/>
-      <c r="D351" s="53"/>
-      <c r="E351" s="53"/>
-      <c r="F351" s="54"/>
+      <c r="A351" s="55" t="s">
+        <v>426</v>
+      </c>
+      <c r="B351" s="55"/>
+      <c r="C351" s="55"/>
+      <c r="D351" s="55"/>
+      <c r="E351" s="55"/>
+      <c r="F351" s="56"/>
     </row>
     <row r="352" spans="1:7">
       <c r="C352" s="13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D352" s="13" t="s">
         <v>5</v>
@@ -15074,7 +15074,7 @@
         <v>116</v>
       </c>
       <c r="F354" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="355" spans="1:6">
@@ -15088,7 +15088,7 @@
         <v>183</v>
       </c>
       <c r="F355" s="14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -15102,7 +15102,7 @@
         <v>182</v>
       </c>
       <c r="F356" s="14" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -15113,10 +15113,10 @@
         <v>4</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F357" s="14" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -15127,44 +15127,44 @@
         <v>4</v>
       </c>
       <c r="C358" s="13" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D358" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E358" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F358" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="359" spans="1:6">
       <c r="A359" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B359" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C359" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="F359" s="14" t="s">
         <v>655</v>
-      </c>
-      <c r="F359" s="14" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="360" spans="1:6">
       <c r="A360" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B360" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C360" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="F360" s="14" t="s">
         <v>657</v>
-      </c>
-      <c r="F360" s="14" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="362" spans="1:6">
@@ -15206,7 +15206,7 @@
         <v>204</v>
       </c>
       <c r="F364" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="365" spans="1:6">
@@ -15220,7 +15220,7 @@
         <v>205</v>
       </c>
       <c r="F365" s="14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="366" spans="1:6">
@@ -15340,7 +15340,7 @@
         <v>125</v>
       </c>
       <c r="F376" s="14" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="377" spans="1:6">
@@ -15364,7 +15364,7 @@
         <v>130</v>
       </c>
       <c r="F379" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="380" spans="1:6">
@@ -15391,7 +15391,7 @@
         <v>135</v>
       </c>
       <c r="F384" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="385" spans="1:6">
@@ -15407,7 +15407,7 @@
         <v>186</v>
       </c>
       <c r="F386" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="387" spans="1:6">
@@ -15415,7 +15415,7 @@
         <v>190</v>
       </c>
       <c r="F387" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="388" spans="1:6">
@@ -15426,7 +15426,7 @@
         <v>5</v>
       </c>
       <c r="E388" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F388" s="14" t="s">
         <v>137</v>
@@ -15434,7 +15434,7 @@
     </row>
     <row r="389" spans="1:6">
       <c r="A389" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B389" s="1" t="s">
         <v>4</v>
@@ -15448,203 +15448,203 @@
     </row>
     <row r="390" spans="1:6">
       <c r="A390" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B390" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F390" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="391" spans="1:6">
       <c r="A391" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B391" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F391" s="14" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="392" spans="1:6">
       <c r="A392" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B392" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C392" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F392" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="395" spans="1:6" ht="27" thickBot="1">
-      <c r="A395" s="53" t="s">
-        <v>255</v>
-      </c>
-      <c r="B395" s="53"/>
-      <c r="C395" s="53"/>
-      <c r="D395" s="53"/>
-      <c r="E395" s="53"/>
-      <c r="F395" s="54"/>
+      <c r="A395" s="55" t="s">
+        <v>254</v>
+      </c>
+      <c r="B395" s="55"/>
+      <c r="C395" s="55"/>
+      <c r="D395" s="55"/>
+      <c r="E395" s="55"/>
+      <c r="F395" s="56"/>
     </row>
     <row r="396" spans="1:6">
       <c r="C396" s="1" t="s">
-        <v>216</v>
+        <v>663</v>
       </c>
       <c r="D396" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E396" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F396" s="14" t="s">
         <v>217</v>
-      </c>
-      <c r="F396" s="14" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="397" spans="1:6">
       <c r="C397" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="F397" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="398" spans="1:6">
       <c r="C398" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F398" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="399" spans="1:6">
       <c r="C399" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F399" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="400" spans="1:6">
       <c r="C400" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F400" s="14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="401" spans="1:6">
       <c r="C401" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="F401" s="14" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="402" spans="1:6">
       <c r="C402" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="F402" s="14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="403" spans="1:6">
       <c r="C403" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="F403" s="14" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="404" spans="1:6">
       <c r="C404" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F404" s="14" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="405" spans="1:6">
       <c r="C405" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F405" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="F405" s="14" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="406" spans="1:6">
       <c r="C406" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="F406" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="F406" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="408" spans="1:6">
       <c r="C408" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="F408" s="14" t="s">
         <v>247</v>
-      </c>
-      <c r="F408" s="14" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="409" spans="1:6">
       <c r="C409" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F409" s="14" t="s">
         <v>249</v>
-      </c>
-      <c r="F409" s="14" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="410" spans="1:6">
       <c r="C410" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="F410" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="F410" s="14" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="411" spans="1:6">
       <c r="C411" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="F411" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="F411" s="14" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="413" spans="1:6">
       <c r="C413" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="416" spans="1:6" ht="27" thickBot="1">
-      <c r="A416" s="53" t="s">
-        <v>264</v>
-      </c>
-      <c r="B416" s="53"/>
-      <c r="C416" s="53"/>
-      <c r="D416" s="53"/>
-      <c r="E416" s="53"/>
-      <c r="F416" s="54"/>
+      <c r="A416" s="55" t="s">
+        <v>263</v>
+      </c>
+      <c r="B416" s="55"/>
+      <c r="C416" s="55"/>
+      <c r="D416" s="55"/>
+      <c r="E416" s="55"/>
+      <c r="F416" s="56"/>
     </row>
     <row r="417" spans="1:6">
       <c r="C417" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F417" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="418" spans="1:6">
@@ -15655,7 +15655,7 @@
     </row>
     <row r="419" spans="1:6">
       <c r="C419" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D419" s="13" t="s">
         <v>5</v>
@@ -15664,7 +15664,7 @@
         <v>23</v>
       </c>
       <c r="F419" s="21" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="420" spans="1:6">
@@ -15678,12 +15678,12 @@
         <v>71</v>
       </c>
       <c r="F420" s="14" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="422" spans="1:6">
       <c r="C422" s="13" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D422" s="13" t="s">
         <v>5</v>
@@ -15692,7 +15692,7 @@
         <v>29</v>
       </c>
       <c r="F422" s="15" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="423" spans="1:6">
@@ -15703,38 +15703,38 @@
         <v>4</v>
       </c>
       <c r="C423" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F423" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="425" spans="1:6">
       <c r="C425" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D425" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E425" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F425" s="22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="426" spans="1:6">
       <c r="C426" s="13" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D426" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E426" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F426" s="21" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="427" spans="1:6">
@@ -15745,10 +15745,10 @@
         <v>4</v>
       </c>
       <c r="C427" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F427" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="428" spans="1:6">
@@ -15759,10 +15759,10 @@
         <v>4</v>
       </c>
       <c r="C428" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F428" s="14" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="429" spans="1:6">
@@ -15773,10 +15773,10 @@
         <v>4</v>
       </c>
       <c r="C429" s="12" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F429" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="430" spans="1:6">
@@ -15787,10 +15787,10 @@
         <v>4</v>
       </c>
       <c r="C430" s="12" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F430" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -15801,10 +15801,10 @@
         <v>4</v>
       </c>
       <c r="C431" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F431" s="14" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="432" spans="1:6">
@@ -15815,10 +15815,10 @@
         <v>4</v>
       </c>
       <c r="C432" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="F432" s="14" t="s">
         <v>534</v>
-      </c>
-      <c r="F432" s="14" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -15829,10 +15829,10 @@
         <v>4</v>
       </c>
       <c r="C433" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F433" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -15843,10 +15843,10 @@
         <v>4</v>
       </c>
       <c r="C434" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F434" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -15857,10 +15857,10 @@
         <v>4</v>
       </c>
       <c r="C435" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F435" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -15874,52 +15874,52 @@
         <v>5</v>
       </c>
       <c r="E437" s="13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F437" s="21" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="438" spans="1:7">
       <c r="A438" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B438" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C438" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F438" s="14" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="439" spans="1:7">
       <c r="A439" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B439" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C439" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F439" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="440" spans="1:7">
       <c r="A440" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B440" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C440" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F440" s="14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -15936,6 +15936,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A416:F416"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A395:F395"/>
     <mergeCell ref="A351:F351"/>
@@ -15943,12 +15949,6 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
-    <mergeCell ref="A416:F416"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds the optional 'filename's to the commit command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82142844-792C-EF47-8851-13CDB0FDFC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1767C04-0258-5348-9D32-C06AC055D2BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26180" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
@@ -5180,20 +5180,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">git commit </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>required option</t>
-    </r>
-  </si>
-  <si>
     <t>Add</t>
   </si>
   <si>
@@ -10295,6 +10281,37 @@
         <rFont val="Menlo Regular"/>
       </rPr>
       <t xml:space="preserve"> --interactive)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git commit </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>filename filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>required option</t>
     </r>
   </si>
 </sst>
@@ -10749,12 +10766,12 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11075,8 +11092,8 @@
   </sheetPr>
   <dimension ref="A1:G445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="168" zoomScaleNormal="168" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="C397" sqref="C397"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="168" zoomScaleNormal="168" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C127" sqref="C127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11113,7 +11130,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -11124,7 +11141,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -11135,7 +11152,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -11146,28 +11163,28 @@
         <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="54"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -11175,25 +11192,25 @@
         <v>44</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="55"/>
-      <c r="C13" s="55"/>
-      <c r="D13" s="55"/>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>5</v>
@@ -11202,12 +11219,12 @@
         <v>1</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="C15" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>5</v>
@@ -11216,12 +11233,12 @@
         <v>2</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="C16" s="13" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>5</v>
@@ -11230,7 +11247,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -11241,12 +11258,12 @@
         <v>4</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="32" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -11260,7 +11277,7 @@
         <v>55</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -11274,7 +11291,7 @@
         <v>54</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -11285,10 +11302,10 @@
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="F20" s="14" t="s">
         <v>485</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>486</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -11299,10 +11316,10 @@
         <v>4</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="F21" s="14" t="s">
         <v>651</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -11313,10 +11330,10 @@
         <v>4</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="F22" s="14" t="s">
         <v>487</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -11330,7 +11347,7 @@
         <v>52</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -11344,7 +11361,7 @@
         <v>191</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -11355,10 +11372,10 @@
         <v>4</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -11372,7 +11389,7 @@
         <v>7</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -11386,7 +11403,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -11400,29 +11417,29 @@
         <v>53</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="C29" s="1" t="s">
+        <v>598</v>
+      </c>
+      <c r="F29" s="14" t="s">
         <v>599</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="17">
       <c r="A30" s="33" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F30" s="14" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -11434,16 +11451,16 @@
       <c r="D32" s="13"/>
       <c r="E32" s="13"/>
       <c r="F32" s="21" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="33"/>
       <c r="C33" s="35" t="s">
+        <v>604</v>
+      </c>
+      <c r="F33" s="31" t="s">
         <v>605</v>
-      </c>
-      <c r="F33" s="31" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -11453,7 +11470,7 @@
     <row r="35" spans="1:6" ht="20" thickBot="1">
       <c r="A35" s="33"/>
       <c r="C35" s="36" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D35" s="37"/>
       <c r="E35" s="37"/>
@@ -11465,25 +11482,25 @@
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="21" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="33"/>
       <c r="C37" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="F37" s="14" t="s">
         <v>609</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="33"/>
       <c r="C38" s="39" t="s">
+        <v>610</v>
+      </c>
+      <c r="F38" s="14" t="s">
         <v>611</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -11497,43 +11514,43 @@
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="21" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="33"/>
       <c r="C41" s="41" t="s">
+        <v>613</v>
+      </c>
+      <c r="F41" s="14" t="s">
         <v>614</v>
-      </c>
-      <c r="F41" s="14" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="33"/>
       <c r="C42" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="F42" s="14" t="s">
         <v>616</v>
-      </c>
-      <c r="F42" s="14" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="33"/>
       <c r="C43" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="F43" s="14" t="s">
         <v>618</v>
-      </c>
-      <c r="F43" s="14" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="40">
       <c r="A44" s="33"/>
       <c r="C44" s="39" t="s">
+        <v>619</v>
+      </c>
+      <c r="F44" s="42" t="s">
         <v>620</v>
-      </c>
-      <c r="F44" s="42" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -11543,10 +11560,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="33"/>
-      <c r="C46" s="57" t="s">
-        <v>622</v>
-      </c>
-      <c r="D46" s="58"/>
+      <c r="C46" s="55" t="s">
+        <v>621</v>
+      </c>
+      <c r="D46" s="56"/>
       <c r="E46" s="37"/>
       <c r="F46" s="43"/>
     </row>
@@ -11556,52 +11573,52 @@
       <c r="D47" s="45"/>
       <c r="E47" s="45"/>
       <c r="F47" s="46" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="33"/>
       <c r="C48" s="41" t="s">
+        <v>613</v>
+      </c>
+      <c r="F48" s="14" t="s">
         <v>614</v>
-      </c>
-      <c r="F48" s="14" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="33"/>
       <c r="C49" s="4" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F49" s="14" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="33"/>
       <c r="C50" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="F50" s="14" t="s">
         <v>625</v>
-      </c>
-      <c r="F50" s="14" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="40">
       <c r="A51" s="33"/>
       <c r="C51" s="39" t="s">
+        <v>626</v>
+      </c>
+      <c r="F51" s="42" t="s">
         <v>627</v>
-      </c>
-      <c r="F51" s="42" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="40">
       <c r="A52" s="33"/>
       <c r="C52" s="39" t="s">
+        <v>628</v>
+      </c>
+      <c r="F52" s="42" t="s">
         <v>629</v>
-      </c>
-      <c r="F52" s="42" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -11612,7 +11629,7 @@
     <row r="54" spans="1:6" ht="20" thickBot="1">
       <c r="A54" s="33"/>
       <c r="C54" s="36" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D54" s="37"/>
       <c r="E54" s="37"/>
@@ -11624,52 +11641,52 @@
       <c r="D55" s="13"/>
       <c r="E55" s="13"/>
       <c r="F55" s="21" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="27">
       <c r="A56" s="33"/>
       <c r="C56" s="51" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F56" s="47" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="33"/>
       <c r="C57" s="39" t="s">
+        <v>632</v>
+      </c>
+      <c r="F57" s="42" t="s">
         <v>633</v>
-      </c>
-      <c r="F57" s="42" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="33"/>
       <c r="C58" s="39" t="s">
+        <v>634</v>
+      </c>
+      <c r="F58" s="42" t="s">
         <v>635</v>
-      </c>
-      <c r="F58" s="42" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="26">
       <c r="A59" s="33"/>
       <c r="C59" s="50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F59" s="49" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="40">
       <c r="A60" s="33"/>
       <c r="C60" s="41" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F60" s="47" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -11683,25 +11700,25 @@
       <c r="D62" s="13"/>
       <c r="E62" s="13"/>
       <c r="F62" s="21" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="27">
       <c r="A63" s="33"/>
       <c r="C63" s="48" t="s">
+        <v>641</v>
+      </c>
+      <c r="F63" s="47" t="s">
         <v>642</v>
-      </c>
-      <c r="F63" s="47" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="26">
       <c r="A64" s="33"/>
       <c r="C64" s="50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F64" s="49" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -11715,25 +11732,25 @@
       <c r="D66" s="13"/>
       <c r="E66" s="13"/>
       <c r="F66" s="21" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="27">
       <c r="A67" s="33"/>
       <c r="C67" s="52" t="s">
+        <v>647</v>
+      </c>
+      <c r="F67" s="47" t="s">
         <v>648</v>
-      </c>
-      <c r="F67" s="47" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="26">
       <c r="A68" s="33"/>
       <c r="C68" s="50" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F68" s="49" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -11742,21 +11759,21 @@
       <c r="F69" s="49"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="55" t="s">
+      <c r="A70" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="55"/>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="55"/>
-      <c r="F70" s="56"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="54"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F71" s="14" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -11764,15 +11781,15 @@
         <v>155</v>
       </c>
       <c r="F72" s="14" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="C73" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F73" s="14" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -11780,7 +11797,7 @@
         <v>154</v>
       </c>
       <c r="F74" s="14" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -11788,7 +11805,7 @@
         <v>10</v>
       </c>
       <c r="F75" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -11796,7 +11813,7 @@
         <v>11</v>
       </c>
       <c r="F76" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -11804,7 +11821,7 @@
         <v>12</v>
       </c>
       <c r="F77" s="14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -11812,7 +11829,7 @@
         <v>13</v>
       </c>
       <c r="F78" s="14" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -11820,15 +11837,15 @@
         <v>109</v>
       </c>
       <c r="F79" s="14" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="17">
       <c r="C80" s="9" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F80" s="14" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -11836,15 +11853,15 @@
         <v>51</v>
       </c>
       <c r="F81" s="14" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="C82" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="F82" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -11852,7 +11869,7 @@
         <v>65</v>
       </c>
       <c r="F83" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -11860,7 +11877,7 @@
         <v>156</v>
       </c>
       <c r="F84" s="14" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -11868,28 +11885,28 @@
         <v>157</v>
       </c>
       <c r="F85" s="14" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="55" t="s">
+      <c r="A87" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="55"/>
-      <c r="C87" s="55"/>
-      <c r="D87" s="55"/>
-      <c r="E87" s="55"/>
-      <c r="F87" s="56"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="54"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F88" s="14" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -11897,7 +11914,7 @@
         <v>18</v>
       </c>
       <c r="F89" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -11905,7 +11922,7 @@
         <v>19</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -11913,7 +11930,7 @@
         <v>293</v>
       </c>
       <c r="F91" s="14" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -11921,7 +11938,7 @@
         <v>294</v>
       </c>
       <c r="F92" s="14" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -11929,7 +11946,7 @@
         <v>295</v>
       </c>
       <c r="F93" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -11937,7 +11954,7 @@
         <v>296</v>
       </c>
       <c r="F94" s="14" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -11945,7 +11962,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="14" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -11953,18 +11970,18 @@
         <v>25</v>
       </c>
       <c r="F96" s="14" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="55" t="s">
+      <c r="A98" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="55"/>
-      <c r="C98" s="55"/>
-      <c r="D98" s="55"/>
-      <c r="E98" s="55"/>
-      <c r="F98" s="55"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
@@ -12051,7 +12068,7 @@
         <v>206</v>
       </c>
       <c r="F109" s="14" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -12105,7 +12122,7 @@
         <v>306</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -12194,7 +12211,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="13" t="s">
-        <v>368</v>
+        <v>663</v>
       </c>
       <c r="D124" s="13" t="s">
         <v>5</v>
@@ -12203,7 +12220,7 @@
         <v>26</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -12294,26 +12311,26 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="55" t="s">
+      <c r="A132" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="55"/>
-      <c r="C132" s="55"/>
-      <c r="D132" s="55"/>
-      <c r="E132" s="55"/>
-      <c r="F132" s="56"/>
+      <c r="B132" s="53"/>
+      <c r="C132" s="53"/>
+      <c r="D132" s="53"/>
+      <c r="E132" s="53"/>
+      <c r="F132" s="54"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
         <v>86</v>
       </c>
       <c r="F133" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="135" spans="1:6">
       <c r="C135" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D135" s="13" t="s">
         <v>5</v>
@@ -12350,7 +12367,7 @@
         <v>184</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -12378,7 +12395,7 @@
         <v>70</v>
       </c>
       <c r="F139" s="14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -12425,7 +12442,7 @@
         <v>62</v>
       </c>
       <c r="F143" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -12439,7 +12456,7 @@
         <v>60</v>
       </c>
       <c r="F144" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -12453,7 +12470,7 @@
         <v>61</v>
       </c>
       <c r="F145" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="146" spans="1:6">
@@ -12464,10 +12481,10 @@
         <v>4</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="F146" s="14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -12481,7 +12498,7 @@
         <v>59</v>
       </c>
       <c r="F147" s="14" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -12495,7 +12512,7 @@
         <v>58</v>
       </c>
       <c r="F148" s="14" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -12509,7 +12526,7 @@
         <v>57</v>
       </c>
       <c r="F149" s="14" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -12523,7 +12540,7 @@
         <v>56</v>
       </c>
       <c r="F150" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -12565,7 +12582,7 @@
         <v>292</v>
       </c>
       <c r="F153" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -12593,7 +12610,7 @@
         <v>1</v>
       </c>
       <c r="F156" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -12607,7 +12624,7 @@
         <v>38</v>
       </c>
       <c r="F157" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="158" spans="1:6">
@@ -12621,7 +12638,7 @@
         <v>1</v>
       </c>
       <c r="F158" s="22" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -12635,7 +12652,7 @@
         <v>39</v>
       </c>
       <c r="F159" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -12649,7 +12666,7 @@
         <v>40</v>
       </c>
       <c r="F160" s="15" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -12663,7 +12680,7 @@
         <v>85</v>
       </c>
       <c r="F161" s="14" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -12677,7 +12694,7 @@
         <v>87</v>
       </c>
       <c r="F162" s="14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -12688,10 +12705,10 @@
         <v>4</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="F163" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -12705,7 +12722,7 @@
         <v>88</v>
       </c>
       <c r="F164" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="165" spans="1:6">
@@ -12719,7 +12736,7 @@
         <v>89</v>
       </c>
       <c r="F165" s="14" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="166" spans="1:6">
@@ -12730,10 +12747,10 @@
         <v>4</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F166" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="167" spans="1:6">
@@ -12747,7 +12764,7 @@
         <v>90</v>
       </c>
       <c r="F167" s="14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -12761,7 +12778,7 @@
         <v>91</v>
       </c>
       <c r="F168" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -12772,10 +12789,10 @@
         <v>4</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F169" s="14" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="170" spans="1:6">
@@ -12789,7 +12806,7 @@
         <v>92</v>
       </c>
       <c r="F170" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -12803,7 +12820,7 @@
         <v>93</v>
       </c>
       <c r="F171" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -12817,7 +12834,7 @@
         <v>94</v>
       </c>
       <c r="F172" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -12831,7 +12848,7 @@
         <v>95</v>
       </c>
       <c r="F173" s="14" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -12842,10 +12859,10 @@
         <v>4</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F174" s="14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="175" spans="1:6">
@@ -12856,10 +12873,10 @@
         <v>4</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F175" s="14" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -12873,7 +12890,7 @@
         <v>200</v>
       </c>
       <c r="F176" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -12887,7 +12904,7 @@
         <v>201</v>
       </c>
       <c r="F177" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="178" spans="1:6">
@@ -12901,54 +12918,54 @@
         <v>202</v>
       </c>
       <c r="F178" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="180" spans="1:6">
       <c r="C180" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D180" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E180" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="F180" s="21" t="s">
         <v>417</v>
-      </c>
-      <c r="F180" s="21" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C181" s="8" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F181" s="14" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="182" spans="1:6">
       <c r="A182" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C182" s="8" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F182" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="183" spans="1:6">
       <c r="A183" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>4</v>
@@ -12957,12 +12974,12 @@
         <v>308</v>
       </c>
       <c r="F183" s="14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="184" spans="1:6">
       <c r="A184" s="1" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>4</v>
@@ -12971,7 +12988,7 @@
         <v>307</v>
       </c>
       <c r="F184" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -12985,7 +13002,7 @@
         <v>306</v>
       </c>
       <c r="F186" s="22" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -12999,7 +13016,7 @@
         <v>73</v>
       </c>
       <c r="F187" s="27" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -13013,7 +13030,7 @@
         <v>302</v>
       </c>
       <c r="F188" s="22" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -13027,7 +13044,7 @@
         <v>298</v>
       </c>
       <c r="F189" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -13041,7 +13058,7 @@
         <v>299</v>
       </c>
       <c r="F190" s="14" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -13055,7 +13072,7 @@
         <v>300</v>
       </c>
       <c r="F191" s="14" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -13069,7 +13086,7 @@
         <v>301</v>
       </c>
       <c r="F192" s="14" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -13083,7 +13100,7 @@
         <v>304</v>
       </c>
       <c r="F193" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -13094,31 +13111,31 @@
         <v>4</v>
       </c>
       <c r="C194" s="5" t="s">
+        <v>496</v>
+      </c>
+      <c r="F194" s="14" t="s">
         <v>497</v>
-      </c>
-      <c r="F194" s="14" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="195" spans="1:6">
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="55" t="s">
-        <v>425</v>
-      </c>
-      <c r="B196" s="55"/>
-      <c r="C196" s="55"/>
-      <c r="D196" s="55"/>
-      <c r="E196" s="55"/>
-      <c r="F196" s="55"/>
+      <c r="A196" s="53" t="s">
+        <v>424</v>
+      </c>
+      <c r="B196" s="53"/>
+      <c r="C196" s="53"/>
+      <c r="D196" s="53"/>
+      <c r="E196" s="53"/>
+      <c r="F196" s="53"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
         <v>256</v>
       </c>
       <c r="F197" s="28" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -13149,7 +13166,7 @@
         <v>239</v>
       </c>
       <c r="F200" s="14" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="201" spans="1:6">
@@ -13163,7 +13180,7 @@
         <v>257</v>
       </c>
       <c r="F201" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -13171,7 +13188,7 @@
     </row>
     <row r="203" spans="1:6">
       <c r="C203" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D203" s="13" t="s">
         <v>5</v>
@@ -13180,7 +13197,7 @@
         <v>262</v>
       </c>
       <c r="F203" s="21" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -13197,10 +13214,10 @@
         <v>5</v>
       </c>
       <c r="E204" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F204" s="14" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -13217,10 +13234,10 @@
         <v>5</v>
       </c>
       <c r="E205" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F205" s="14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -13237,10 +13254,10 @@
         <v>5</v>
       </c>
       <c r="E206" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F206" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -13251,16 +13268,16 @@
         <v>4</v>
       </c>
       <c r="C207" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D207" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E207" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F207" s="14" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -13277,10 +13294,10 @@
         <v>5</v>
       </c>
       <c r="E208" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F208" s="14" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="209" spans="1:6">
@@ -13291,44 +13308,44 @@
         <v>4</v>
       </c>
       <c r="C209" s="24" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D209" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E209" s="13" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F209" s="15" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="210" spans="1:6">
       <c r="A210" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C210" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F210" s="14" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="211" spans="1:6">
       <c r="A211" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C211" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F211" s="14" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="212" spans="1:6">
@@ -13336,49 +13353,49 @@
     </row>
     <row r="213" spans="1:6">
       <c r="C213" s="13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D213" s="13" t="s">
         <v>5</v>
       </c>
       <c r="E213" s="13" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F213" s="21" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="214" spans="1:6">
       <c r="A214" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C214" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F214" s="14" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="215" spans="1:6">
       <c r="A215" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C215" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F215" s="14" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="216" spans="1:6">
       <c r="A216" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>4</v>
@@ -13387,21 +13404,21 @@
         <v>265</v>
       </c>
       <c r="F216" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="217" spans="1:6">
       <c r="A217" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C217" s="8" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="F217" s="14" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="219" spans="1:6">
@@ -13415,7 +13432,7 @@
         <v>1</v>
       </c>
       <c r="F219" s="21" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="220" spans="1:6">
@@ -13429,7 +13446,7 @@
         <v>101</v>
       </c>
       <c r="F220" s="14" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -13443,7 +13460,7 @@
         <v>102</v>
       </c>
       <c r="F221" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -13499,7 +13516,7 @@
         <v>105</v>
       </c>
       <c r="F225" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -13513,7 +13530,7 @@
         <v>106</v>
       </c>
       <c r="F226" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -13527,7 +13544,7 @@
         <v>107</v>
       </c>
       <c r="F227" s="14" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -13541,7 +13558,7 @@
         <v>108</v>
       </c>
       <c r="F228" s="14" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -13577,7 +13594,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="C232" s="24" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D232" s="13" t="s">
         <v>5</v>
@@ -13598,7 +13615,7 @@
         <v>194</v>
       </c>
       <c r="F233" s="14" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -13612,7 +13629,7 @@
         <v>196</v>
       </c>
       <c r="F234" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -13626,7 +13643,7 @@
         <v>195</v>
       </c>
       <c r="F235" s="14" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -13640,7 +13657,7 @@
         <v>203</v>
       </c>
       <c r="F236" s="14" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -13651,7 +13668,7 @@
         <v>4</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D237" s="13" t="s">
         <v>5</v>
@@ -13674,7 +13691,7 @@
         <v>197</v>
       </c>
       <c r="F238" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -13702,28 +13719,28 @@
         <v>199</v>
       </c>
       <c r="F240" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="242" spans="1:7" ht="27" thickBot="1">
-      <c r="A242" s="55" t="s">
-        <v>585</v>
-      </c>
-      <c r="B242" s="55"/>
-      <c r="C242" s="55"/>
-      <c r="D242" s="55"/>
-      <c r="E242" s="55"/>
-      <c r="F242" s="56"/>
+      <c r="A242" s="53" t="s">
+        <v>584</v>
+      </c>
+      <c r="B242" s="53"/>
+      <c r="C242" s="53"/>
+      <c r="D242" s="53"/>
+      <c r="E242" s="53"/>
+      <c r="F242" s="54"/>
     </row>
     <row r="243" spans="1:7">
       <c r="C243" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F243" s="14" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="G243" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="244" spans="1:7">
@@ -13734,7 +13751,7 @@
         <v>321</v>
       </c>
       <c r="G244" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="245" spans="1:7">
@@ -13745,7 +13762,7 @@
         <v>322</v>
       </c>
       <c r="G245" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="246" spans="1:7">
@@ -13756,7 +13773,7 @@
         <v>323</v>
       </c>
       <c r="G246" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="247" spans="1:7">
@@ -13767,7 +13784,7 @@
         <v>324</v>
       </c>
       <c r="G247" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="249" spans="1:7">
@@ -13781,10 +13798,10 @@
         <v>28</v>
       </c>
       <c r="F249" s="14" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="250" spans="1:7">
@@ -13798,10 +13815,10 @@
         <v>32</v>
       </c>
       <c r="F250" s="14" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="251" spans="1:7">
@@ -13812,13 +13829,13 @@
         <v>4</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F251" s="14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="252" spans="1:7">
@@ -13829,13 +13846,13 @@
         <v>4</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F252" s="14" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="253" spans="1:7">
@@ -13849,61 +13866,61 @@
         <v>168</v>
       </c>
       <c r="F253" s="14" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="255" spans="1:7">
       <c r="C255" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D255" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E255" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="F255" s="22" t="s">
+        <v>548</v>
+      </c>
+      <c r="G255" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="F255" s="22" t="s">
-        <v>549</v>
-      </c>
-      <c r="G255" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="256" spans="1:7">
       <c r="A256" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B256" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C256" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="F256" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="G256" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C256" s="30" t="s">
-        <v>548</v>
-      </c>
-      <c r="F256" s="14" t="s">
-        <v>575</v>
-      </c>
-      <c r="G256" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="257" spans="1:7">
       <c r="A257" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C257" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="F257" s="14" t="s">
+        <v>583</v>
+      </c>
+      <c r="G257" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>552</v>
-      </c>
-      <c r="F257" s="14" t="s">
-        <v>584</v>
-      </c>
-      <c r="G257" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="258" spans="1:7">
@@ -13920,7 +13937,7 @@
         <v>40</v>
       </c>
       <c r="F259" s="14" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G259" s="1"/>
     </row>
@@ -13983,13 +14000,13 @@
         <v>4</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F263" s="14" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G263" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="264" spans="1:7">
@@ -14000,13 +14017,13 @@
         <v>4</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F264" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G264" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="265" spans="1:7">
@@ -14023,7 +14040,7 @@
         <v>315</v>
       </c>
       <c r="G265" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="266" spans="1:7">
@@ -14034,13 +14051,13 @@
         <v>4</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F266" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G266" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="267" spans="1:7">
@@ -14057,7 +14074,7 @@
         <v>243</v>
       </c>
       <c r="G267" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="268" spans="1:7">
@@ -14083,7 +14100,7 @@
         <v>144</v>
       </c>
       <c r="F273" s="14" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="274" spans="1:7">
@@ -14145,13 +14162,13 @@
         <v>4</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F277" s="14" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G277" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="278" spans="1:7">
@@ -14162,13 +14179,13 @@
         <v>4</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F278" s="14" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G278" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="279" spans="1:7">
@@ -14185,7 +14202,7 @@
         <v>315</v>
       </c>
       <c r="G279" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="280" spans="1:7">
@@ -14196,13 +14213,13 @@
         <v>4</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F280" s="14" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G280" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="281" spans="1:7">
@@ -14219,7 +14236,7 @@
         <v>243</v>
       </c>
       <c r="G281" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="284" spans="1:7">
@@ -14233,7 +14250,7 @@
         <v>144</v>
       </c>
       <c r="F284" s="14" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="285" spans="1:7">
@@ -14247,7 +14264,7 @@
         <v>144</v>
       </c>
       <c r="F285" s="14" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="286" spans="1:7">
@@ -14261,7 +14278,7 @@
         <v>172</v>
       </c>
       <c r="F286" s="14" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="287" spans="1:7">
@@ -14275,7 +14292,7 @@
         <v>173</v>
       </c>
       <c r="F287" s="14" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="288" spans="1:7">
@@ -14289,7 +14306,7 @@
         <v>174</v>
       </c>
       <c r="F288" s="14" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="289" spans="1:7">
@@ -14306,10 +14323,10 @@
         <v>29</v>
       </c>
       <c r="F290" s="22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="291" spans="1:7">
@@ -14323,10 +14340,10 @@
         <v>87</v>
       </c>
       <c r="F291" s="14" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="292" spans="1:7">
@@ -14340,10 +14357,10 @@
         <v>82</v>
       </c>
       <c r="F292" s="14" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="293" spans="1:7">
@@ -14357,10 +14374,10 @@
         <v>83</v>
       </c>
       <c r="F293" s="14" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="294" spans="1:7">
@@ -14374,10 +14391,10 @@
         <v>84</v>
       </c>
       <c r="F294" s="14" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="295" spans="1:7">
@@ -14391,10 +14408,10 @@
         <v>240</v>
       </c>
       <c r="F295" s="14" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="296" spans="1:7">
@@ -14405,13 +14422,13 @@
         <v>4</v>
       </c>
       <c r="C296" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="F296" s="14" t="s">
         <v>587</v>
       </c>
-      <c r="F296" s="14" t="s">
-        <v>588</v>
-      </c>
       <c r="G296" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="297" spans="1:7">
@@ -14425,10 +14442,10 @@
         <v>283</v>
       </c>
       <c r="F297" s="14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="301" spans="1:7">
@@ -14438,14 +14455,14 @@
       <c r="C302" s="2"/>
     </row>
     <row r="304" spans="1:7" ht="27" thickBot="1">
-      <c r="A304" s="55" t="s">
+      <c r="A304" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="B304" s="55"/>
-      <c r="C304" s="55"/>
-      <c r="D304" s="55"/>
-      <c r="E304" s="55"/>
-      <c r="F304" s="56"/>
+      <c r="B304" s="53"/>
+      <c r="C304" s="53"/>
+      <c r="D304" s="53"/>
+      <c r="E304" s="53"/>
+      <c r="F304" s="54"/>
     </row>
     <row r="307" spans="1:6">
       <c r="C307" s="1" t="s">
@@ -14657,7 +14674,7 @@
         <v>75</v>
       </c>
       <c r="G321" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="322" spans="1:7">
@@ -14674,7 +14691,7 @@
         <v>75</v>
       </c>
       <c r="G322" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="323" spans="1:7">
@@ -14691,7 +14708,7 @@
         <v>76</v>
       </c>
       <c r="G323" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="324" spans="1:7">
@@ -14708,7 +14725,7 @@
         <v>141</v>
       </c>
       <c r="G324" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="325" spans="1:7">
@@ -14719,13 +14736,13 @@
         <v>4</v>
       </c>
       <c r="C325" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F325" s="14" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G325" s="9" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="326" spans="1:7">
@@ -14736,10 +14753,10 @@
         <v>4</v>
       </c>
       <c r="C326" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F326" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G326" s="9" t="s">
         <v>295</v>
@@ -14759,7 +14776,7 @@
         <v>315</v>
       </c>
       <c r="G327" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="328" spans="1:7">
@@ -14807,10 +14824,10 @@
         <v>144</v>
       </c>
       <c r="F331" s="14" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="332" spans="1:7">
@@ -14827,7 +14844,7 @@
         <v>75</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="333" spans="1:7">
@@ -14844,7 +14861,7 @@
         <v>76</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="334" spans="1:7">
@@ -14861,7 +14878,7 @@
         <v>141</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="335" spans="1:7">
@@ -14872,13 +14889,13 @@
         <v>4</v>
       </c>
       <c r="C335" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F335" s="14" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="336" spans="1:7">
@@ -14889,10 +14906,10 @@
         <v>4</v>
       </c>
       <c r="C336" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F336" s="14" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G336" s="1" t="s">
         <v>295</v>
@@ -14912,7 +14929,7 @@
         <v>315</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="338" spans="1:7">
@@ -14954,7 +14971,7 @@
         <v>77</v>
       </c>
       <c r="F340" s="14" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="341" spans="1:7">
@@ -14962,7 +14979,7 @@
         <v>78</v>
       </c>
       <c r="F341" s="14" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="343" spans="1:7">
@@ -15026,18 +15043,18 @@
       </c>
     </row>
     <row r="351" spans="1:7" ht="27" thickBot="1">
-      <c r="A351" s="55" t="s">
-        <v>426</v>
-      </c>
-      <c r="B351" s="55"/>
-      <c r="C351" s="55"/>
-      <c r="D351" s="55"/>
-      <c r="E351" s="55"/>
-      <c r="F351" s="56"/>
+      <c r="A351" s="53" t="s">
+        <v>425</v>
+      </c>
+      <c r="B351" s="53"/>
+      <c r="C351" s="53"/>
+      <c r="D351" s="53"/>
+      <c r="E351" s="53"/>
+      <c r="F351" s="54"/>
     </row>
     <row r="352" spans="1:7">
       <c r="C352" s="13" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D352" s="13" t="s">
         <v>5</v>
@@ -15088,7 +15105,7 @@
         <v>183</v>
       </c>
       <c r="F355" s="14" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="356" spans="1:6">
@@ -15102,7 +15119,7 @@
         <v>182</v>
       </c>
       <c r="F356" s="14" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="357" spans="1:6">
@@ -15113,10 +15130,10 @@
         <v>4</v>
       </c>
       <c r="C357" s="2" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F357" s="14" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="358" spans="1:6">
@@ -15127,7 +15144,7 @@
         <v>4</v>
       </c>
       <c r="C358" s="13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D358" s="13" t="s">
         <v>5</v>
@@ -15136,7 +15153,7 @@
         <v>302</v>
       </c>
       <c r="F358" s="21" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="359" spans="1:6">
@@ -15147,10 +15164,10 @@
         <v>4</v>
       </c>
       <c r="C359" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="F359" s="14" t="s">
         <v>654</v>
-      </c>
-      <c r="F359" s="14" t="s">
-        <v>655</v>
       </c>
     </row>
     <row r="360" spans="1:6">
@@ -15161,10 +15178,10 @@
         <v>4</v>
       </c>
       <c r="C360" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="F360" s="14" t="s">
         <v>656</v>
-      </c>
-      <c r="F360" s="14" t="s">
-        <v>657</v>
       </c>
     </row>
     <row r="362" spans="1:6">
@@ -15454,7 +15471,7 @@
         <v>4</v>
       </c>
       <c r="C390" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F390" s="14" t="s">
         <v>276</v>
@@ -15468,7 +15485,7 @@
         <v>4</v>
       </c>
       <c r="C391" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F391" s="14" t="s">
         <v>277</v>
@@ -15482,25 +15499,25 @@
         <v>4</v>
       </c>
       <c r="C392" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F392" s="14" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="395" spans="1:6" ht="27" thickBot="1">
-      <c r="A395" s="55" t="s">
+      <c r="A395" s="53" t="s">
         <v>254</v>
       </c>
-      <c r="B395" s="55"/>
-      <c r="C395" s="55"/>
-      <c r="D395" s="55"/>
-      <c r="E395" s="55"/>
-      <c r="F395" s="56"/>
+      <c r="B395" s="53"/>
+      <c r="C395" s="53"/>
+      <c r="D395" s="53"/>
+      <c r="E395" s="53"/>
+      <c r="F395" s="54"/>
     </row>
     <row r="396" spans="1:6">
       <c r="C396" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D396" s="1" t="s">
         <v>5</v>
@@ -15630,21 +15647,21 @@
       </c>
     </row>
     <row r="416" spans="1:6" ht="27" thickBot="1">
-      <c r="A416" s="55" t="s">
+      <c r="A416" s="53" t="s">
         <v>263</v>
       </c>
-      <c r="B416" s="55"/>
-      <c r="C416" s="55"/>
-      <c r="D416" s="55"/>
-      <c r="E416" s="55"/>
-      <c r="F416" s="56"/>
+      <c r="B416" s="53"/>
+      <c r="C416" s="53"/>
+      <c r="D416" s="53"/>
+      <c r="E416" s="53"/>
+      <c r="F416" s="54"/>
     </row>
     <row r="417" spans="1:6">
       <c r="C417" s="1" t="s">
         <v>269</v>
       </c>
       <c r="F417" s="14" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="418" spans="1:6">
@@ -15655,7 +15672,7 @@
     </row>
     <row r="419" spans="1:6">
       <c r="C419" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D419" s="13" t="s">
         <v>5</v>
@@ -15664,7 +15681,7 @@
         <v>23</v>
       </c>
       <c r="F419" s="21" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="420" spans="1:6">
@@ -15683,7 +15700,7 @@
     </row>
     <row r="422" spans="1:6">
       <c r="C422" s="13" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D422" s="13" t="s">
         <v>5</v>
@@ -15692,7 +15709,7 @@
         <v>29</v>
       </c>
       <c r="F422" s="15" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="423" spans="1:6">
@@ -15706,7 +15723,7 @@
         <v>283</v>
       </c>
       <c r="F423" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="425" spans="1:6">
@@ -15725,7 +15742,7 @@
     </row>
     <row r="426" spans="1:6">
       <c r="C426" s="13" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D426" s="13" t="s">
         <v>5</v>
@@ -15734,7 +15751,7 @@
         <v>274</v>
       </c>
       <c r="F426" s="21" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="427" spans="1:6">
@@ -15748,7 +15765,7 @@
         <v>267</v>
       </c>
       <c r="F427" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="428" spans="1:6">
@@ -15762,7 +15779,7 @@
         <v>268</v>
       </c>
       <c r="F428" s="14" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="429" spans="1:6">
@@ -15776,7 +15793,7 @@
         <v>275</v>
       </c>
       <c r="F429" s="14" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="430" spans="1:6">
@@ -15790,7 +15807,7 @@
         <v>272</v>
       </c>
       <c r="F430" s="14" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="431" spans="1:6">
@@ -15804,7 +15821,7 @@
         <v>273</v>
       </c>
       <c r="F431" s="14" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="432" spans="1:6">
@@ -15815,10 +15832,10 @@
         <v>4</v>
       </c>
       <c r="C432" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="F432" s="14" t="s">
         <v>533</v>
-      </c>
-      <c r="F432" s="14" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="433" spans="1:7">
@@ -15832,7 +15849,7 @@
         <v>271</v>
       </c>
       <c r="F433" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="434" spans="1:7">
@@ -15846,7 +15863,7 @@
         <v>265</v>
       </c>
       <c r="F434" s="14" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="435" spans="1:7">
@@ -15860,7 +15877,7 @@
         <v>266</v>
       </c>
       <c r="F435" s="14" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="436" spans="1:7">
@@ -15877,7 +15894,7 @@
         <v>282</v>
       </c>
       <c r="F437" s="21" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="438" spans="1:7">
@@ -15891,7 +15908,7 @@
         <v>279</v>
       </c>
       <c r="F438" s="14" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="439" spans="1:7">
@@ -15905,7 +15922,7 @@
         <v>280</v>
       </c>
       <c r="F439" s="14" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="440" spans="1:7">
@@ -15919,7 +15936,7 @@
         <v>281</v>
       </c>
       <c r="F440" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="442" spans="1:7">
@@ -15936,12 +15953,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A416:F416"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A395:F395"/>
     <mergeCell ref="A351:F351"/>
@@ -15949,6 +15960,12 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
+    <mergeCell ref="A416:F416"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Clarifies the description for the 'add origin' command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D482197-0875-9649-BE63-65ADBABBF94A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422AB42-B92A-9140-BD33-837B67FFA902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="26820" yWindow="480" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10548,24 +10548,72 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Create a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>new remote</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> named </t>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (delete) a remote branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Rename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a remote branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>repo URL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a new remote branch named </t>
     </r>
     <r>
       <rPr>
@@ -10584,58 +10632,15 @@
         <rFont val="Arial Narrow"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> (convention)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Remove</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (delete) a remote branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Rename</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a remote branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Update a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>repo URL</t>
+      <t xml:space="preserve"> (convention) to an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>empty repo</t>
     </r>
   </si>
 </sst>
@@ -11089,12 +11094,12 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11415,8 +11420,8 @@
   </sheetPr>
   <dimension ref="A1:F427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A270" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="A295" sqref="A295:XFD297"/>
+    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="F341" sqref="F341"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11493,14 +11498,14 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="56"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
@@ -11522,14 +11527,14 @@
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="53"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
@@ -11883,10 +11888,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="32"/>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="54" t="s">
         <v>607</v>
       </c>
-      <c r="D46" s="57"/>
+      <c r="D46" s="55"/>
       <c r="E46" s="36"/>
       <c r="F46" s="42"/>
     </row>
@@ -12082,14 +12087,14 @@
       <c r="F69" s="48"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="55"/>
+      <c r="B70" s="52"/>
+      <c r="C70" s="52"/>
+      <c r="D70" s="52"/>
+      <c r="E70" s="52"/>
+      <c r="F70" s="53"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
@@ -12215,14 +12220,14 @@
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="54" t="s">
+      <c r="A87" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="54"/>
-      <c r="C87" s="54"/>
-      <c r="D87" s="54"/>
-      <c r="E87" s="54"/>
-      <c r="F87" s="55"/>
+      <c r="B87" s="52"/>
+      <c r="C87" s="52"/>
+      <c r="D87" s="52"/>
+      <c r="E87" s="52"/>
+      <c r="F87" s="53"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
@@ -12297,14 +12302,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="54" t="s">
+      <c r="A98" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="54"/>
-      <c r="C98" s="54"/>
-      <c r="D98" s="54"/>
-      <c r="E98" s="54"/>
-      <c r="F98" s="54"/>
+      <c r="B98" s="52"/>
+      <c r="C98" s="52"/>
+      <c r="D98" s="52"/>
+      <c r="E98" s="52"/>
+      <c r="F98" s="52"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
@@ -12634,14 +12639,14 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="54" t="s">
+      <c r="A132" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="54"/>
-      <c r="C132" s="54"/>
-      <c r="D132" s="54"/>
-      <c r="E132" s="54"/>
-      <c r="F132" s="55"/>
+      <c r="B132" s="52"/>
+      <c r="C132" s="52"/>
+      <c r="D132" s="52"/>
+      <c r="E132" s="52"/>
+      <c r="F132" s="53"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
@@ -13444,14 +13449,14 @@
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="54" t="s">
+      <c r="A196" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="54"/>
-      <c r="C196" s="54"/>
-      <c r="D196" s="54"/>
-      <c r="E196" s="54"/>
-      <c r="F196" s="54"/>
+      <c r="B196" s="52"/>
+      <c r="C196" s="52"/>
+      <c r="D196" s="52"/>
+      <c r="E196" s="52"/>
+      <c r="F196" s="52"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
@@ -14046,14 +14051,14 @@
       </c>
     </row>
     <row r="242" spans="1:6" ht="27" thickBot="1">
-      <c r="A242" s="54" t="s">
+      <c r="A242" s="52" t="s">
         <v>573</v>
       </c>
-      <c r="B242" s="54"/>
-      <c r="C242" s="54"/>
-      <c r="D242" s="54"/>
-      <c r="E242" s="54"/>
-      <c r="F242" s="55"/>
+      <c r="B242" s="52"/>
+      <c r="C242" s="52"/>
+      <c r="D242" s="52"/>
+      <c r="E242" s="52"/>
+      <c r="F242" s="53"/>
     </row>
     <row r="243" spans="1:6">
       <c r="C243" s="1" t="s">
@@ -14619,14 +14624,14 @@
       </c>
     </row>
     <row r="291" spans="1:6" ht="27" thickBot="1">
-      <c r="A291" s="54" t="s">
+      <c r="A291" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="B291" s="54"/>
-      <c r="C291" s="54"/>
-      <c r="D291" s="54"/>
-      <c r="E291" s="54"/>
-      <c r="F291" s="55"/>
+      <c r="B291" s="52"/>
+      <c r="C291" s="52"/>
+      <c r="D291" s="52"/>
+      <c r="E291" s="52"/>
+      <c r="F291" s="53"/>
     </row>
     <row r="292" spans="1:6">
       <c r="C292" s="1" t="s">
@@ -15153,14 +15158,14 @@
       </c>
     </row>
     <row r="340" spans="1:6" ht="27" thickBot="1">
-      <c r="A340" s="54" t="s">
+      <c r="A340" s="52" t="s">
         <v>421</v>
       </c>
-      <c r="B340" s="54"/>
-      <c r="C340" s="54"/>
-      <c r="D340" s="54"/>
-      <c r="E340" s="54"/>
-      <c r="F340" s="55"/>
+      <c r="B340" s="52"/>
+      <c r="C340" s="52"/>
+      <c r="D340" s="52"/>
+      <c r="E340" s="52"/>
+      <c r="F340" s="53"/>
     </row>
     <row r="341" spans="1:6">
       <c r="C341" s="13" t="s">
@@ -15201,7 +15206,7 @@
         <v>115</v>
       </c>
       <c r="F343" s="14" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -15215,7 +15220,7 @@
         <v>180</v>
       </c>
       <c r="F344" s="14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -15229,7 +15234,7 @@
         <v>179</v>
       </c>
       <c r="F345" s="14" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -15243,7 +15248,7 @@
         <v>643</v>
       </c>
       <c r="F346" s="14" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -15613,14 +15618,14 @@
       </c>
     </row>
     <row r="382" spans="1:6" ht="27" thickBot="1">
-      <c r="A382" s="54" t="s">
+      <c r="A382" s="52" t="s">
         <v>251</v>
       </c>
-      <c r="B382" s="54"/>
-      <c r="C382" s="54"/>
-      <c r="D382" s="54"/>
-      <c r="E382" s="54"/>
-      <c r="F382" s="55"/>
+      <c r="B382" s="52"/>
+      <c r="C382" s="52"/>
+      <c r="D382" s="52"/>
+      <c r="E382" s="52"/>
+      <c r="F382" s="53"/>
     </row>
     <row r="383" spans="1:6">
       <c r="C383" s="1" t="s">
@@ -15754,14 +15759,14 @@
       </c>
     </row>
     <row r="403" spans="1:6" ht="27" thickBot="1">
-      <c r="A403" s="54" t="s">
+      <c r="A403" s="52" t="s">
         <v>260</v>
       </c>
-      <c r="B403" s="54"/>
-      <c r="C403" s="54"/>
-      <c r="D403" s="54"/>
-      <c r="E403" s="54"/>
-      <c r="F403" s="55"/>
+      <c r="B403" s="52"/>
+      <c r="C403" s="52"/>
+      <c r="D403" s="52"/>
+      <c r="E403" s="52"/>
+      <c r="F403" s="53"/>
     </row>
     <row r="404" spans="1:6">
       <c r="C404" s="1" t="s">
@@ -16048,12 +16053,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A403:F403"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A382:F382"/>
     <mergeCell ref="A340:F340"/>
@@ -16061,6 +16060,12 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
+    <mergeCell ref="A403:F403"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Adds a 'set-upstream-to=origin' command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E422AB42-B92A-9140-BD33-837B67FFA902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F25868C-F611-264F-B991-DE3BCC83FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="480" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="26820" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$98:$F$379</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$98:$F$380</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <webPublishing allowPng="1" targetScreenSize="1024x768" codePage="10000"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="675">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="676">
   <si>
     <t>Configuration</t>
   </si>
@@ -10641,6 +10641,37 @@
         <rFont val="Menlo Bold"/>
       </rPr>
       <t>empty repo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>git branch --set-upstream-to=</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>origin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>branch_name branch_name</t>
     </r>
   </si>
 </sst>
@@ -11023,7 +11054,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -11094,12 +11125,15 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11418,10 +11452,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F427"/>
+  <dimension ref="A1:F428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A328" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="F341" sqref="F341"/>
+    <sheetView tabSelected="1" topLeftCell="A351" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C373" sqref="C373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11498,14 +11532,14 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="57"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
@@ -11527,14 +11561,14 @@
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="52"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="B13" s="54"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="54"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
@@ -11888,10 +11922,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="32"/>
-      <c r="C46" s="54" t="s">
+      <c r="C46" s="56" t="s">
         <v>607</v>
       </c>
-      <c r="D46" s="55"/>
+      <c r="D46" s="57"/>
       <c r="E46" s="36"/>
       <c r="F46" s="42"/>
     </row>
@@ -12087,14 +12121,14 @@
       <c r="F69" s="48"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="52" t="s">
+      <c r="A70" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="52"/>
-      <c r="C70" s="52"/>
-      <c r="D70" s="52"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="53"/>
+      <c r="B70" s="54"/>
+      <c r="C70" s="54"/>
+      <c r="D70" s="54"/>
+      <c r="E70" s="54"/>
+      <c r="F70" s="55"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
@@ -12220,14 +12254,14 @@
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="52" t="s">
+      <c r="A87" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="52"/>
-      <c r="C87" s="52"/>
-      <c r="D87" s="52"/>
-      <c r="E87" s="52"/>
-      <c r="F87" s="53"/>
+      <c r="B87" s="54"/>
+      <c r="C87" s="54"/>
+      <c r="D87" s="54"/>
+      <c r="E87" s="54"/>
+      <c r="F87" s="55"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
@@ -12302,14 +12336,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="52" t="s">
+      <c r="A98" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="52"/>
-      <c r="C98" s="52"/>
-      <c r="D98" s="52"/>
-      <c r="E98" s="52"/>
-      <c r="F98" s="52"/>
+      <c r="B98" s="54"/>
+      <c r="C98" s="54"/>
+      <c r="D98" s="54"/>
+      <c r="E98" s="54"/>
+      <c r="F98" s="54"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
@@ -12639,14 +12673,14 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="52" t="s">
+      <c r="A132" s="54" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="52"/>
-      <c r="C132" s="52"/>
-      <c r="D132" s="52"/>
-      <c r="E132" s="52"/>
-      <c r="F132" s="53"/>
+      <c r="B132" s="54"/>
+      <c r="C132" s="54"/>
+      <c r="D132" s="54"/>
+      <c r="E132" s="54"/>
+      <c r="F132" s="55"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
@@ -13449,14 +13483,14 @@
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="52" t="s">
+      <c r="A196" s="54" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="52"/>
-      <c r="C196" s="52"/>
-      <c r="D196" s="52"/>
-      <c r="E196" s="52"/>
-      <c r="F196" s="52"/>
+      <c r="B196" s="54"/>
+      <c r="C196" s="54"/>
+      <c r="D196" s="54"/>
+      <c r="E196" s="54"/>
+      <c r="F196" s="54"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
@@ -14051,14 +14085,14 @@
       </c>
     </row>
     <row r="242" spans="1:6" ht="27" thickBot="1">
-      <c r="A242" s="52" t="s">
+      <c r="A242" s="54" t="s">
         <v>573</v>
       </c>
-      <c r="B242" s="52"/>
-      <c r="C242" s="52"/>
-      <c r="D242" s="52"/>
-      <c r="E242" s="52"/>
-      <c r="F242" s="53"/>
+      <c r="B242" s="54"/>
+      <c r="C242" s="54"/>
+      <c r="D242" s="54"/>
+      <c r="E242" s="54"/>
+      <c r="F242" s="55"/>
     </row>
     <row r="243" spans="1:6">
       <c r="C243" s="1" t="s">
@@ -14624,14 +14658,14 @@
       </c>
     </row>
     <row r="291" spans="1:6" ht="27" thickBot="1">
-      <c r="A291" s="52" t="s">
+      <c r="A291" s="54" t="s">
         <v>111</v>
       </c>
-      <c r="B291" s="52"/>
-      <c r="C291" s="52"/>
-      <c r="D291" s="52"/>
-      <c r="E291" s="52"/>
-      <c r="F291" s="53"/>
+      <c r="B291" s="54"/>
+      <c r="C291" s="54"/>
+      <c r="D291" s="54"/>
+      <c r="E291" s="54"/>
+      <c r="F291" s="55"/>
     </row>
     <row r="292" spans="1:6">
       <c r="C292" s="1" t="s">
@@ -15158,14 +15192,14 @@
       </c>
     </row>
     <row r="340" spans="1:6" ht="27" thickBot="1">
-      <c r="A340" s="52" t="s">
+      <c r="A340" s="54" t="s">
         <v>421</v>
       </c>
-      <c r="B340" s="52"/>
-      <c r="C340" s="52"/>
-      <c r="D340" s="52"/>
-      <c r="E340" s="52"/>
-      <c r="F340" s="53"/>
+      <c r="B340" s="54"/>
+      <c r="C340" s="54"/>
+      <c r="D340" s="54"/>
+      <c r="E340" s="54"/>
+      <c r="F340" s="55"/>
     </row>
     <row r="341" spans="1:6">
       <c r="C341" s="13" t="s">
@@ -15491,85 +15525,79 @@
         <v>123</v>
       </c>
     </row>
-    <row r="367" spans="1:6">
-      <c r="C367" s="3" t="s">
+    <row r="367" spans="1:6" ht="27">
+      <c r="C367" s="58" t="s">
+        <v>675</v>
+      </c>
+      <c r="F367" s="41" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6">
+      <c r="C368" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="F367" s="14" t="s">
+      <c r="F368" s="14" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="368" spans="1:6">
-      <c r="C368" s="4" t="s">
+    <row r="369" spans="1:6">
+      <c r="C369" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="F368" s="14" t="s">
+      <c r="F369" s="14" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="369" spans="1:6">
-      <c r="C369" s="1" t="s">
+    <row r="370" spans="1:6">
+      <c r="C370" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="F369" s="14" t="s">
+      <c r="F370" s="14" t="s">
         <v>140</v>
-      </c>
-    </row>
-    <row r="371" spans="1:6">
-      <c r="C371" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="F371" s="14" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="372" spans="1:6">
       <c r="C372" s="1" t="s">
-        <v>205</v>
+        <v>134</v>
       </c>
       <c r="F372" s="14" t="s">
-        <v>206</v>
+        <v>315</v>
       </c>
     </row>
     <row r="373" spans="1:6">
       <c r="C373" s="1" t="s">
-        <v>183</v>
+        <v>205</v>
       </c>
       <c r="F373" s="14" t="s">
-        <v>315</v>
+        <v>206</v>
       </c>
     </row>
     <row r="374" spans="1:6">
       <c r="C374" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F374" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="375" spans="1:6">
       <c r="C375" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F375" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6">
+      <c r="C376" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D375" s="1" t="s">
+      <c r="D376" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E375" s="1" t="s">
+      <c r="E376" s="1" t="s">
         <v>279</v>
-      </c>
-      <c r="F375" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="376" spans="1:6">
-      <c r="A376" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B376" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C376" s="3" t="s">
-        <v>181</v>
       </c>
       <c r="F376" s="14" t="s">
         <v>136</v>
@@ -15582,11 +15610,11 @@
       <c r="B377" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C377" s="1" t="s">
-        <v>531</v>
+      <c r="C377" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="F377" s="14" t="s">
-        <v>273</v>
+        <v>136</v>
       </c>
     </row>
     <row r="378" spans="1:6">
@@ -15596,11 +15624,11 @@
       <c r="B378" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C378" s="3" t="s">
-        <v>532</v>
+      <c r="C378" s="1" t="s">
+        <v>531</v>
       </c>
       <c r="F378" s="14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="379" spans="1:6">
@@ -15611,273 +15639,273 @@
         <v>4</v>
       </c>
       <c r="C379" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="F379" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6">
+      <c r="A380" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B380" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C380" s="3" t="s">
         <v>533</v>
       </c>
-      <c r="F379" s="14" t="s">
+      <c r="F380" s="14" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="382" spans="1:6" ht="27" thickBot="1">
-      <c r="A382" s="52" t="s">
+    <row r="383" spans="1:6" ht="27" thickBot="1">
+      <c r="A383" s="54" t="s">
         <v>251</v>
       </c>
-      <c r="B382" s="52"/>
-      <c r="C382" s="52"/>
-      <c r="D382" s="52"/>
-      <c r="E382" s="52"/>
-      <c r="F382" s="53"/>
-    </row>
-    <row r="383" spans="1:6">
-      <c r="C383" s="1" t="s">
-        <v>648</v>
-      </c>
-      <c r="D383" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E383" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="F383" s="14" t="s">
-        <v>214</v>
-      </c>
+      <c r="B383" s="54"/>
+      <c r="C383" s="54"/>
+      <c r="D383" s="54"/>
+      <c r="E383" s="54"/>
+      <c r="F383" s="55"/>
     </row>
     <row r="384" spans="1:6">
       <c r="C384" s="1" t="s">
-        <v>217</v>
+        <v>648</v>
+      </c>
+      <c r="D384" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E384" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="F384" s="14" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
     </row>
     <row r="385" spans="3:6">
       <c r="C385" s="1" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F385" s="14" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="386" spans="3:6">
       <c r="C386" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F386" s="14" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="387" spans="3:6">
       <c r="C387" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F387" s="14" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="388" spans="3:6">
       <c r="C388" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F388" s="14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="389" spans="3:6">
       <c r="C389" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F389" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="390" spans="3:6">
       <c r="C390" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F390" s="14" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="391" spans="3:6">
       <c r="C391" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="F391" s="14" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="392" spans="3:6">
+      <c r="C392" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="F391" s="14" t="s">
+      <c r="F392" s="14" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="392" spans="3:6">
-      <c r="C392" s="3" t="s">
+    <row r="393" spans="3:6">
+      <c r="C393" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F392" s="14" t="s">
+      <c r="F393" s="14" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="393" spans="3:6">
-      <c r="C393" s="1" t="s">
+    <row r="394" spans="3:6">
+      <c r="C394" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F393" s="14" t="s">
+      <c r="F394" s="14" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="395" spans="3:6">
-      <c r="C395" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="F395" s="14" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="396" spans="3:6">
       <c r="C396" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F396" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="397" spans="3:6">
       <c r="C397" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F397" s="14" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="398" spans="3:6">
       <c r="C398" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F398" s="14" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="399" spans="3:6">
+      <c r="C399" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F398" s="14" t="s">
+      <c r="F399" s="14" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="400" spans="3:6">
-      <c r="C400" s="1" t="s">
+    <row r="401" spans="1:6">
+      <c r="C401" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="403" spans="1:6" ht="27" thickBot="1">
-      <c r="A403" s="52" t="s">
+    <row r="404" spans="1:6" ht="27" thickBot="1">
+      <c r="A404" s="54" t="s">
         <v>260</v>
       </c>
-      <c r="B403" s="52"/>
-      <c r="C403" s="52"/>
-      <c r="D403" s="52"/>
-      <c r="E403" s="52"/>
-      <c r="F403" s="53"/>
-    </row>
-    <row r="404" spans="1:6">
-      <c r="C404" s="1" t="s">
+      <c r="B404" s="54"/>
+      <c r="C404" s="54"/>
+      <c r="D404" s="54"/>
+      <c r="E404" s="54"/>
+      <c r="F404" s="55"/>
+    </row>
+    <row r="405" spans="1:6">
+      <c r="C405" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="F404" s="14" t="s">
+      <c r="F405" s="14" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="405" spans="1:6">
-      <c r="C405" s="25"/>
-      <c r="D405" s="25"/>
-      <c r="E405" s="25"/>
-      <c r="F405" s="27"/>
-    </row>
     <row r="406" spans="1:6">
-      <c r="C406" s="13" t="s">
+      <c r="C406" s="25"/>
+      <c r="D406" s="25"/>
+      <c r="E406" s="25"/>
+      <c r="F406" s="27"/>
+    </row>
+    <row r="407" spans="1:6">
+      <c r="C407" s="13" t="s">
         <v>366</v>
       </c>
-      <c r="D406" s="13" t="s">
+      <c r="D407" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E406" s="13" t="s">
+      <c r="E407" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F406" s="21" t="s">
+      <c r="F407" s="21" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="407" spans="1:6">
-      <c r="A407" s="1" t="s">
+    <row r="408" spans="1:6">
+      <c r="A408" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B407" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C407" s="3" t="s">
+      <c r="B408" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C408" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F407" s="14" t="s">
+      <c r="F408" s="14" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="409" spans="1:6">
-      <c r="C409" s="13" t="s">
+    <row r="410" spans="1:6">
+      <c r="C410" s="13" t="s">
         <v>525</v>
       </c>
-      <c r="D409" s="13" t="s">
+      <c r="D410" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E409" s="13" t="s">
+      <c r="E410" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F409" s="15" t="s">
+      <c r="F410" s="15" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="410" spans="1:6">
-      <c r="A410" s="1" t="s">
+    <row r="411" spans="1:6">
+      <c r="A411" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B410" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C410" s="8" t="s">
+      <c r="B411" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C411" s="8" t="s">
         <v>280</v>
       </c>
-      <c r="F410" s="14" t="s">
+      <c r="F411" s="14" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="412" spans="1:6">
-      <c r="C412" s="1" t="s">
+    <row r="413" spans="1:6">
+      <c r="C413" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="D412" s="1" t="s">
+      <c r="D413" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E412" s="1" t="s">
+      <c r="E413" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="F412" s="22" t="s">
+      <c r="F413" s="22" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="413" spans="1:6">
-      <c r="C413" s="13" t="s">
+    <row r="414" spans="1:6">
+      <c r="C414" s="13" t="s">
         <v>519</v>
       </c>
-      <c r="D413" s="13" t="s">
+      <c r="D414" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E413" s="13" t="s">
+      <c r="E414" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="F413" s="21" t="s">
+      <c r="F414" s="21" t="s">
         <v>518</v>
-      </c>
-    </row>
-    <row r="414" spans="1:6">
-      <c r="A414" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B414" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C414" s="10" t="s">
-        <v>264</v>
-      </c>
-      <c r="F414" s="14" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="415" spans="1:6">
@@ -15887,11 +15915,11 @@
       <c r="B415" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C415" s="2" t="s">
-        <v>265</v>
+      <c r="C415" s="10" t="s">
+        <v>264</v>
       </c>
       <c r="F415" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="416" spans="1:6">
@@ -15901,11 +15929,11 @@
       <c r="B416" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C416" s="12" t="s">
-        <v>272</v>
+      <c r="C416" s="2" t="s">
+        <v>265</v>
       </c>
       <c r="F416" s="14" t="s">
-        <v>530</v>
+        <v>515</v>
       </c>
     </row>
     <row r="417" spans="1:6">
@@ -15916,10 +15944,10 @@
         <v>4</v>
       </c>
       <c r="C417" s="12" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F417" s="14" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
     </row>
     <row r="418" spans="1:6">
@@ -15930,10 +15958,10 @@
         <v>4</v>
       </c>
       <c r="C418" s="12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F418" s="14" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
     </row>
     <row r="419" spans="1:6">
@@ -15943,11 +15971,11 @@
       <c r="B419" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C419" s="8" t="s">
-        <v>528</v>
+      <c r="C419" s="12" t="s">
+        <v>270</v>
       </c>
       <c r="F419" s="14" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="420" spans="1:6">
@@ -15958,10 +15986,10 @@
         <v>4</v>
       </c>
       <c r="C420" s="8" t="s">
-        <v>268</v>
+        <v>528</v>
       </c>
       <c r="F420" s="14" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
     </row>
     <row r="421" spans="1:6">
@@ -15972,10 +16000,10 @@
         <v>4</v>
       </c>
       <c r="C421" s="8" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="F421" s="14" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="422" spans="1:6">
@@ -15986,41 +16014,41 @@
         <v>4</v>
       </c>
       <c r="C422" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="F422" s="14" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6">
+      <c r="A423" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B423" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C423" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="F422" s="14" t="s">
+      <c r="F423" s="14" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="423" spans="1:6">
-      <c r="C423" s="8"/>
-    </row>
     <row r="424" spans="1:6">
-      <c r="C424" s="24" t="s">
+      <c r="C424" s="8"/>
+    </row>
+    <row r="425" spans="1:6">
+      <c r="C425" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="D424" s="13" t="s">
+      <c r="D425" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E424" s="13" t="s">
+      <c r="E425" s="13" t="s">
         <v>279</v>
       </c>
-      <c r="F424" s="21" t="s">
+      <c r="F425" s="21" t="s">
         <v>534</v>
-      </c>
-    </row>
-    <row r="425" spans="1:6">
-      <c r="A425" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B425" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C425" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F425" s="14" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="426" spans="1:6">
@@ -16031,10 +16059,10 @@
         <v>4</v>
       </c>
       <c r="C426" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F426" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="427" spans="1:6">
@@ -16045,27 +16073,41 @@
         <v>4</v>
       </c>
       <c r="C427" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F427" s="14" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6">
+      <c r="A428" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B428" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C428" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="F427" s="14" t="s">
+      <c r="F428" s="14" t="s">
         <v>537</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A404:F404"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A382:F382"/>
+    <mergeCell ref="A383:F383"/>
     <mergeCell ref="A340:F340"/>
     <mergeCell ref="A291:F291"/>
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
-    <mergeCell ref="A403:F403"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Updates the '.ods' file with changes made to '.xlsx' file.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F25868C-F611-264F-B991-DE3BCC83FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE6DC5D-263D-DF4A-9772-C6DA2730F7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26820" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
@@ -11455,7 +11455,7 @@
   <dimension ref="A1:F428"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A351" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="C373" sqref="C373"/>
+      <selection activeCell="C367" sqref="C367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Corrects 'Stop' to 'Start' for the 'set-upstream' command.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE6DC5D-263D-DF4A-9772-C6DA2730F7FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0254F479-A29A-DF44-9931-EAE376C311CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26820" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="676">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="677">
   <si>
     <t>Configuration</t>
   </si>
@@ -10673,6 +10673,9 @@
       </rPr>
       <t>branch_name branch_name</t>
     </r>
+  </si>
+  <si>
+    <t>Start tracking a remote repo</t>
   </si>
 </sst>
 </file>
@@ -11125,15 +11128,15 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11455,7 +11458,7 @@
   <dimension ref="A1:F428"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A351" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="C367" sqref="C367"/>
+      <selection activeCell="F367" sqref="F367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11532,14 +11535,14 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="52" t="s">
+      <c r="A9" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="52"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="B9" s="57"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="58"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
@@ -11561,14 +11564,14 @@
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="55"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="53"/>
+      <c r="F13" s="54"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
@@ -11922,10 +11925,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="32"/>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="55" t="s">
         <v>607</v>
       </c>
-      <c r="D46" s="57"/>
+      <c r="D46" s="56"/>
       <c r="E46" s="36"/>
       <c r="F46" s="42"/>
     </row>
@@ -12121,14 +12124,14 @@
       <c r="F69" s="48"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="54"/>
-      <c r="C70" s="54"/>
-      <c r="D70" s="54"/>
-      <c r="E70" s="54"/>
-      <c r="F70" s="55"/>
+      <c r="B70" s="53"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="53"/>
+      <c r="E70" s="53"/>
+      <c r="F70" s="54"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
@@ -12254,14 +12257,14 @@
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="54" t="s">
+      <c r="A87" s="53" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="54"/>
-      <c r="C87" s="54"/>
-      <c r="D87" s="54"/>
-      <c r="E87" s="54"/>
-      <c r="F87" s="55"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="54"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
@@ -12336,14 +12339,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="54" t="s">
+      <c r="A98" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="54"/>
-      <c r="C98" s="54"/>
-      <c r="D98" s="54"/>
-      <c r="E98" s="54"/>
-      <c r="F98" s="54"/>
+      <c r="B98" s="53"/>
+      <c r="C98" s="53"/>
+      <c r="D98" s="53"/>
+      <c r="E98" s="53"/>
+      <c r="F98" s="53"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
@@ -12673,14 +12676,14 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="54" t="s">
+      <c r="A132" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="54"/>
-      <c r="C132" s="54"/>
-      <c r="D132" s="54"/>
-      <c r="E132" s="54"/>
-      <c r="F132" s="55"/>
+      <c r="B132" s="53"/>
+      <c r="C132" s="53"/>
+      <c r="D132" s="53"/>
+      <c r="E132" s="53"/>
+      <c r="F132" s="54"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
@@ -13483,14 +13486,14 @@
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="54" t="s">
+      <c r="A196" s="53" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="54"/>
-      <c r="C196" s="54"/>
-      <c r="D196" s="54"/>
-      <c r="E196" s="54"/>
-      <c r="F196" s="54"/>
+      <c r="B196" s="53"/>
+      <c r="C196" s="53"/>
+      <c r="D196" s="53"/>
+      <c r="E196" s="53"/>
+      <c r="F196" s="53"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
@@ -14085,14 +14088,14 @@
       </c>
     </row>
     <row r="242" spans="1:6" ht="27" thickBot="1">
-      <c r="A242" s="54" t="s">
+      <c r="A242" s="53" t="s">
         <v>573</v>
       </c>
-      <c r="B242" s="54"/>
-      <c r="C242" s="54"/>
-      <c r="D242" s="54"/>
-      <c r="E242" s="54"/>
-      <c r="F242" s="55"/>
+      <c r="B242" s="53"/>
+      <c r="C242" s="53"/>
+      <c r="D242" s="53"/>
+      <c r="E242" s="53"/>
+      <c r="F242" s="54"/>
     </row>
     <row r="243" spans="1:6">
       <c r="C243" s="1" t="s">
@@ -14658,14 +14661,14 @@
       </c>
     </row>
     <row r="291" spans="1:6" ht="27" thickBot="1">
-      <c r="A291" s="54" t="s">
+      <c r="A291" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="B291" s="54"/>
-      <c r="C291" s="54"/>
-      <c r="D291" s="54"/>
-      <c r="E291" s="54"/>
-      <c r="F291" s="55"/>
+      <c r="B291" s="53"/>
+      <c r="C291" s="53"/>
+      <c r="D291" s="53"/>
+      <c r="E291" s="53"/>
+      <c r="F291" s="54"/>
     </row>
     <row r="292" spans="1:6">
       <c r="C292" s="1" t="s">
@@ -15192,14 +15195,14 @@
       </c>
     </row>
     <row r="340" spans="1:6" ht="27" thickBot="1">
-      <c r="A340" s="54" t="s">
+      <c r="A340" s="53" t="s">
         <v>421</v>
       </c>
-      <c r="B340" s="54"/>
-      <c r="C340" s="54"/>
-      <c r="D340" s="54"/>
-      <c r="E340" s="54"/>
-      <c r="F340" s="55"/>
+      <c r="B340" s="53"/>
+      <c r="C340" s="53"/>
+      <c r="D340" s="53"/>
+      <c r="E340" s="53"/>
+      <c r="F340" s="54"/>
     </row>
     <row r="341" spans="1:6">
       <c r="C341" s="13" t="s">
@@ -15526,11 +15529,11 @@
       </c>
     </row>
     <row r="367" spans="1:6" ht="27">
-      <c r="C367" s="58" t="s">
+      <c r="C367" s="52" t="s">
         <v>675</v>
       </c>
       <c r="F367" s="41" t="s">
-        <v>307</v>
+        <v>676</v>
       </c>
     </row>
     <row r="368" spans="1:6">
@@ -15660,14 +15663,14 @@
       </c>
     </row>
     <row r="383" spans="1:6" ht="27" thickBot="1">
-      <c r="A383" s="54" t="s">
+      <c r="A383" s="53" t="s">
         <v>251</v>
       </c>
-      <c r="B383" s="54"/>
-      <c r="C383" s="54"/>
-      <c r="D383" s="54"/>
-      <c r="E383" s="54"/>
-      <c r="F383" s="55"/>
+      <c r="B383" s="53"/>
+      <c r="C383" s="53"/>
+      <c r="D383" s="53"/>
+      <c r="E383" s="53"/>
+      <c r="F383" s="54"/>
     </row>
     <row r="384" spans="1:6">
       <c r="C384" s="1" t="s">
@@ -15801,14 +15804,14 @@
       </c>
     </row>
     <row r="404" spans="1:6" ht="27" thickBot="1">
-      <c r="A404" s="54" t="s">
+      <c r="A404" s="53" t="s">
         <v>260</v>
       </c>
-      <c r="B404" s="54"/>
-      <c r="C404" s="54"/>
-      <c r="D404" s="54"/>
-      <c r="E404" s="54"/>
-      <c r="F404" s="55"/>
+      <c r="B404" s="53"/>
+      <c r="C404" s="53"/>
+      <c r="D404" s="53"/>
+      <c r="E404" s="53"/>
+      <c r="F404" s="54"/>
     </row>
     <row r="405" spans="1:6">
       <c r="C405" s="1" t="s">
@@ -16095,12 +16098,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A404:F404"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A383:F383"/>
     <mergeCell ref="A340:F340"/>
@@ -16108,6 +16105,12 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
+    <mergeCell ref="A404:F404"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Corrects the 'Update a repo URL' command ie + 'set-url'.
</commit_message>
<xml_diff>
--- a/git-terminal-commands.xlsx
+++ b/git-terminal-commands.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Goofy/GIT/steves-git-commands/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0254F479-A29A-DF44-9931-EAE376C311CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44901D34-F1A3-D549-ACB8-BD9BBD26F085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26820" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
+    <workbookView xWindow="26800" yWindow="460" windowWidth="24380" windowHeight="28340" xr2:uid="{B9461A18-709B-FF48-BF68-DFA38E1882C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10017,16 +10017,665 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">git tag </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>required option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">(-l </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> --list) </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git remote </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">prune </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git add (-i </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="7" tint="-0.249977111117893"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>OR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> --interactive)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git commit </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>filename filename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>required option</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Switch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (replaces checkout)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move HEAD to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>another branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creates a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>new branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and moves the HEAD to it</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creates a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>new tracking branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and moves the HEAD to it</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">--detached </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>tree-ish</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">-m </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>branch_name</t>
+    </r>
+  </si>
+  <si>
+    <t>Switch and merge working trees</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">--discard-changes </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>branch_name</t>
+    </r>
+  </si>
+  <si>
+    <t>Switch to another branch without saving working files</t>
+  </si>
+  <si>
+    <r>
+      <t>string</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Restore changes from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>commit directly to current work file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create and switch to a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>new branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>tag reference</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>orphaned commit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>tree-ish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (detached HEAD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to another branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>without saving working files</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>merge working trees</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move HEAD to a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>patch of changes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move HEAD to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>another</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Creates a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>new tracking</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> branch and moves the HEAD to it</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create and switch to a new branch from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>tag reference</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>orphaned commit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> from a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>tree-ish</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> reference (detached HEAD)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Show </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>more information</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> of all remotes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Remove</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (delete) a remote branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Rename</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a remote branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>repo URL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>Push</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a new remote branch named </t>
+    </r>
+    <r>
       <rPr>
         <i/>
         <sz val="9"/>
         <color rgb="FFFFC000"/>
-        <rFont val="Menlo Regular"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
       </rPr>
       <t>origin</t>
     </r>
     <r>
       <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (convention) to an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Menlo Bold"/>
+      </rPr>
+      <t>empty repo</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>git branch --set-upstream-to=</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>origin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>/</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color theme="4"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>branch_name branch_name</t>
+    </r>
+  </si>
+  <si>
+    <t>Start tracking a remote repo</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t>set-url</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="9"/>
+        <color rgb="FFFFC000"/>
+        <rFont val="Menlo Regular"/>
+      </rPr>
+      <t xml:space="preserve"> origin</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
         <sz val="9"/>
         <color rgb="FF0070C0"/>
@@ -10034,648 +10683,6 @@
       </rPr>
       <t xml:space="preserve"> remote_url</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git tag </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>required option</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">(-l </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --list) </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>option</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git remote </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>option</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">prune </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>option</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git add (-i </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="7" tint="-0.249977111117893"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>OR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> --interactive)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git commit </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>filename filename</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>required option</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Switch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (replaces checkout)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Move HEAD to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>another branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Creates a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>new branch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and moves the HEAD to it</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Creates a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>new tracking branch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and moves the HEAD to it</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">--detached </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="4"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>tree-ish</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">-m </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="4"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>branch_name</t>
-    </r>
-  </si>
-  <si>
-    <t>Switch and merge working trees</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">--discard-changes </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="4"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>branch_name</t>
-    </r>
-  </si>
-  <si>
-    <t>Switch to another branch without saving working files</t>
-  </si>
-  <si>
-    <r>
-      <t>string</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>*</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Restore changes from a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>commit directly to current work file</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create and switch to a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>new branch</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> from a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>tag reference</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>orphaned commit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> from a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>tree-ish</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> reference</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (detached HEAD)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Switch to another branch </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>without saving working files</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Switch and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>merge working trees</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Move HEAD to a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>patch of changes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Move HEAD to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>another</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Creates a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>new tracking</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> branch and moves the HEAD to it</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create and switch to a new branch from a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>tag reference</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Create an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>orphaned commit</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> from a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>tree-ish</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> reference (detached HEAD)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Show </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>more information</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> of all remotes</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Remove</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (delete) a remote branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Rename</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a remote branch</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Update a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>repo URL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>Push</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a new remote branch named </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t>origin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Arial Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (convention) to an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF7030A0"/>
-        <rFont val="Menlo Bold"/>
-      </rPr>
-      <t>empty repo</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>git branch --set-upstream-to=</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color rgb="FFFFC000"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>origin</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="9"/>
-        <color theme="4"/>
-        <rFont val="Menlo Regular"/>
-      </rPr>
-      <t>branch_name branch_name</t>
-    </r>
-  </si>
-  <si>
-    <t>Start tracking a remote repo</t>
   </si>
 </sst>
 </file>
@@ -11131,12 +11138,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="52" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" xr:uid="{ACEF5201-9FF9-AD44-AA4C-60ABCDBD9D8F}"/>
@@ -11457,8 +11464,8 @@
   </sheetPr>
   <dimension ref="A1:F428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
-      <selection activeCell="F367" sqref="F367"/>
+    <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" zoomScaleSheetLayoutView="33" workbookViewId="0">
+      <selection activeCell="C347" sqref="C347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -11535,14 +11542,14 @@
       <c r="A8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="27" thickBot="1">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="58"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="54"/>
     </row>
     <row r="10" spans="1:6">
       <c r="C10" s="1" t="s">
@@ -11564,14 +11571,14 @@
       <c r="A12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickBot="1">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="54"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
     </row>
     <row r="14" spans="1:6">
       <c r="C14" s="1" t="s">
@@ -11925,10 +11932,10 @@
     </row>
     <row r="46" spans="1:6" ht="20" thickBot="1">
       <c r="A46" s="32"/>
-      <c r="C46" s="55" t="s">
+      <c r="C46" s="57" t="s">
         <v>607</v>
       </c>
-      <c r="D46" s="56"/>
+      <c r="D46" s="58"/>
       <c r="E46" s="36"/>
       <c r="F46" s="42"/>
     </row>
@@ -12124,14 +12131,14 @@
       <c r="F69" s="48"/>
     </row>
     <row r="70" spans="1:6" ht="27" thickBot="1">
-      <c r="A70" s="53" t="s">
+      <c r="A70" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="B70" s="53"/>
-      <c r="C70" s="53"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="54"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="55"/>
+      <c r="D70" s="55"/>
+      <c r="E70" s="55"/>
+      <c r="F70" s="56"/>
     </row>
     <row r="71" spans="1:6">
       <c r="C71" s="1" t="s">
@@ -12257,14 +12264,14 @@
       <c r="A86" s="20"/>
     </row>
     <row r="87" spans="1:6" ht="27" thickBot="1">
-      <c r="A87" s="53" t="s">
+      <c r="A87" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="B87" s="53"/>
-      <c r="C87" s="53"/>
-      <c r="D87" s="53"/>
-      <c r="E87" s="53"/>
-      <c r="F87" s="54"/>
+      <c r="B87" s="55"/>
+      <c r="C87" s="55"/>
+      <c r="D87" s="55"/>
+      <c r="E87" s="55"/>
+      <c r="F87" s="56"/>
     </row>
     <row r="88" spans="1:6">
       <c r="C88" s="1" t="s">
@@ -12339,14 +12346,14 @@
       </c>
     </row>
     <row r="98" spans="1:6" ht="27" thickBot="1">
-      <c r="A98" s="53" t="s">
+      <c r="A98" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B98" s="53"/>
-      <c r="C98" s="53"/>
-      <c r="D98" s="53"/>
-      <c r="E98" s="53"/>
-      <c r="F98" s="53"/>
+      <c r="B98" s="55"/>
+      <c r="C98" s="55"/>
+      <c r="D98" s="55"/>
+      <c r="E98" s="55"/>
+      <c r="F98" s="55"/>
     </row>
     <row r="99" spans="1:6">
       <c r="C99" s="1" t="s">
@@ -12576,7 +12583,7 @@
     </row>
     <row r="124" spans="1:6">
       <c r="C124" s="13" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D124" s="13" t="s">
         <v>5</v>
@@ -12676,14 +12683,14 @@
       <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:6" ht="27" thickBot="1">
-      <c r="A132" s="53" t="s">
+      <c r="A132" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B132" s="53"/>
-      <c r="C132" s="53"/>
-      <c r="D132" s="53"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="54"/>
+      <c r="B132" s="55"/>
+      <c r="C132" s="55"/>
+      <c r="D132" s="55"/>
+      <c r="E132" s="55"/>
+      <c r="F132" s="56"/>
     </row>
     <row r="133" spans="1:6">
       <c r="C133" s="1" t="s">
@@ -13486,14 +13493,14 @@
       <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:6" ht="27" thickBot="1">
-      <c r="A196" s="53" t="s">
+      <c r="A196" s="55" t="s">
         <v>420</v>
       </c>
-      <c r="B196" s="53"/>
-      <c r="C196" s="53"/>
-      <c r="D196" s="53"/>
-      <c r="E196" s="53"/>
-      <c r="F196" s="53"/>
+      <c r="B196" s="55"/>
+      <c r="C196" s="55"/>
+      <c r="D196" s="55"/>
+      <c r="E196" s="55"/>
+      <c r="F196" s="55"/>
     </row>
     <row r="197" spans="1:6">
       <c r="C197" s="8" t="s">
@@ -13959,7 +13966,7 @@
     </row>
     <row r="232" spans="1:6">
       <c r="C232" s="24" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D232" s="13" t="s">
         <v>5</v>
@@ -14033,7 +14040,7 @@
         <v>4</v>
       </c>
       <c r="C237" s="23" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D237" s="13" t="s">
         <v>5</v>
@@ -14088,14 +14095,14 @@
       </c>
     </row>
     <row r="242" spans="1:6" ht="27" thickBot="1">
-      <c r="A242" s="53" t="s">
+      <c r="A242" s="55" t="s">
         <v>573</v>
       </c>
-      <c r="B242" s="53"/>
-      <c r="C242" s="53"/>
-      <c r="D242" s="53"/>
-      <c r="E242" s="53"/>
-      <c r="F242" s="54"/>
+      <c r="B242" s="55"/>
+      <c r="C242" s="55"/>
+      <c r="D242" s="55"/>
+      <c r="E242" s="55"/>
+      <c r="F242" s="56"/>
     </row>
     <row r="243" spans="1:6">
       <c r="C243" s="1" t="s">
@@ -14189,7 +14196,7 @@
         <v>4</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F252" s="14" t="s">
         <v>555</v>
@@ -14262,7 +14269,7 @@
         <v>40</v>
       </c>
       <c r="F259" s="15" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="260" spans="1:6">
@@ -14276,7 +14283,7 @@
         <v>144</v>
       </c>
       <c r="F260" s="14" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="261" spans="1:6">
@@ -14290,7 +14297,7 @@
         <v>173</v>
       </c>
       <c r="F261" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="262" spans="1:6">
@@ -14304,7 +14311,7 @@
         <v>174</v>
       </c>
       <c r="F262" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="263" spans="1:6">
@@ -14318,7 +14325,7 @@
         <v>211</v>
       </c>
       <c r="F263" s="14" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="264" spans="1:6">
@@ -14329,10 +14336,10 @@
         <v>4</v>
       </c>
       <c r="C264" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F264" s="14" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="265" spans="1:6">
@@ -14343,10 +14350,10 @@
         <v>4</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F265" s="14" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="266" spans="1:6">
@@ -14357,10 +14364,10 @@
         <v>4</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F266" s="14" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="267" spans="1:6">
@@ -14374,7 +14381,7 @@
         <v>239</v>
       </c>
       <c r="F267" s="14" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="269" spans="1:6">
@@ -14402,7 +14409,7 @@
         <v>144</v>
       </c>
       <c r="F270" s="14" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="271" spans="1:6">
@@ -14416,7 +14423,7 @@
         <v>145</v>
       </c>
       <c r="F271" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="272" spans="1:6">
@@ -14430,7 +14437,7 @@
         <v>146</v>
       </c>
       <c r="F272" s="14" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="273" spans="1:6">
@@ -14458,7 +14465,7 @@
         <v>550</v>
       </c>
       <c r="F274" s="14" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="275" spans="1:6">
@@ -14472,7 +14479,7 @@
         <v>212</v>
       </c>
       <c r="F275" s="14" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="276" spans="1:6">
@@ -14486,7 +14493,7 @@
         <v>578</v>
       </c>
       <c r="F276" s="14" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="277" spans="1:6">
@@ -14500,7 +14507,7 @@
         <v>239</v>
       </c>
       <c r="F277" s="14" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="278" spans="1:6">
@@ -14661,14 +14668,14 @@
       </c>
     </row>
     <row r="291" spans="1:6" ht="27" thickBot="1">
-      <c r="A291" s="53" t="s">
+      <c r="A291" s="55" t="s">
         <v>111</v>
       </c>
-      <c r="B291" s="53"/>
-      <c r="C291" s="53"/>
-      <c r="D291" s="53"/>
-      <c r="E291" s="53"/>
-      <c r="F291" s="54"/>
+      <c r="B291" s="55"/>
+      <c r="C291" s="55"/>
+      <c r="D291" s="55"/>
+      <c r="E291" s="55"/>
+      <c r="F291" s="56"/>
     </row>
     <row r="292" spans="1:6">
       <c r="C292" s="1" t="s">
@@ -14877,7 +14884,7 @@
         <v>40</v>
       </c>
       <c r="F310" s="14" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="311" spans="1:6">
@@ -14891,7 +14898,7 @@
         <v>144</v>
       </c>
       <c r="F311" s="14" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="312" spans="1:6">
@@ -14905,7 +14912,7 @@
         <v>173</v>
       </c>
       <c r="F312" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="313" spans="1:6">
@@ -14919,7 +14926,7 @@
         <v>174</v>
       </c>
       <c r="F313" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="314" spans="1:6">
@@ -14944,7 +14951,7 @@
         <v>4</v>
       </c>
       <c r="C315" s="3" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F315" s="14" t="s">
         <v>577</v>
@@ -14958,10 +14965,10 @@
         <v>4</v>
       </c>
       <c r="C316" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="F316" s="14" t="s">
         <v>657</v>
-      </c>
-      <c r="F316" s="14" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="317" spans="1:6">
@@ -14972,10 +14979,10 @@
         <v>4</v>
       </c>
       <c r="C317" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="F317" s="14" t="s">
         <v>655</v>
-      </c>
-      <c r="F317" s="14" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="318" spans="1:6">
@@ -15195,18 +15202,18 @@
       </c>
     </row>
     <row r="340" spans="1:6" ht="27" thickBot="1">
-      <c r="A340" s="53" t="s">
+      <c r="A340" s="55" t="s">
         <v>421</v>
       </c>
-      <c r="B340" s="53"/>
-      <c r="C340" s="53"/>
-      <c r="D340" s="53"/>
-      <c r="E340" s="53"/>
-      <c r="F340" s="54"/>
+      <c r="B340" s="55"/>
+      <c r="C340" s="55"/>
+      <c r="D340" s="55"/>
+      <c r="E340" s="55"/>
+      <c r="F340" s="56"/>
     </row>
     <row r="341" spans="1:6">
       <c r="C341" s="13" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D341" s="13" t="s">
         <v>5</v>
@@ -15229,7 +15236,7 @@
         <v>114</v>
       </c>
       <c r="F342" s="14" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="343" spans="1:6">
@@ -15243,7 +15250,7 @@
         <v>115</v>
       </c>
       <c r="F343" s="14" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="344" spans="1:6">
@@ -15257,7 +15264,7 @@
         <v>180</v>
       </c>
       <c r="F344" s="14" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="345" spans="1:6">
@@ -15271,7 +15278,7 @@
         <v>179</v>
       </c>
       <c r="F345" s="14" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="346" spans="1:6">
@@ -15281,11 +15288,11 @@
       <c r="B346" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C346" s="2" t="s">
-        <v>643</v>
+      <c r="C346" s="11" t="s">
+        <v>676</v>
       </c>
       <c r="F346" s="14" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="347" spans="1:6">
@@ -15296,7 +15303,7 @@
         <v>4</v>
       </c>
       <c r="C347" s="13" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D347" s="13" t="s">
         <v>5</v>
@@ -15530,10 +15537,10 @@
     </row>
     <row r="367" spans="1:6" ht="27">
       <c r="C367" s="52" t="s">
+        <v>674</v>
+      </c>
+      <c r="F367" s="41" t="s">
         <v>675</v>
-      </c>
-      <c r="F367" s="41" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="368" spans="1:6">
@@ -15663,18 +15670,18 @@
       </c>
     </row>
     <row r="383" spans="1:6" ht="27" thickBot="1">
-      <c r="A383" s="53" t="s">
+      <c r="A383" s="55" t="s">
         <v>251</v>
       </c>
-      <c r="B383" s="53"/>
-      <c r="C383" s="53"/>
-      <c r="D383" s="53"/>
-      <c r="E383" s="53"/>
-      <c r="F383" s="54"/>
+      <c r="B383" s="55"/>
+      <c r="C383" s="55"/>
+      <c r="D383" s="55"/>
+      <c r="E383" s="55"/>
+      <c r="F383" s="56"/>
     </row>
     <row r="384" spans="1:6">
       <c r="C384" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D384" s="1" t="s">
         <v>5</v>
@@ -15804,14 +15811,14 @@
       </c>
     </row>
     <row r="404" spans="1:6" ht="27" thickBot="1">
-      <c r="A404" s="53" t="s">
+      <c r="A404" s="55" t="s">
         <v>260</v>
       </c>
-      <c r="B404" s="53"/>
-      <c r="C404" s="53"/>
-      <c r="D404" s="53"/>
-      <c r="E404" s="53"/>
-      <c r="F404" s="54"/>
+      <c r="B404" s="55"/>
+      <c r="C404" s="55"/>
+      <c r="D404" s="55"/>
+      <c r="E404" s="55"/>
+      <c r="F404" s="56"/>
     </row>
     <row r="405" spans="1:6">
       <c r="C405" s="1" t="s">
@@ -16098,6 +16105,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A404:F404"/>
+    <mergeCell ref="A98:F98"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A132:F132"/>
+    <mergeCell ref="A70:F70"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="A383:F383"/>
     <mergeCell ref="A340:F340"/>
@@ -16105,12 +16118,6 @@
     <mergeCell ref="A242:F242"/>
     <mergeCell ref="A87:F87"/>
     <mergeCell ref="A196:F196"/>
-    <mergeCell ref="A404:F404"/>
-    <mergeCell ref="A98:F98"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A132:F132"/>
-    <mergeCell ref="A70:F70"/>
-    <mergeCell ref="C46:D46"/>
   </mergeCells>
   <phoneticPr fontId="16" type="noConversion"/>
   <hyperlinks>

</xml_diff>